<commit_message>
Certifications data set to dynamic
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24401"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{230DBF4F-14B3-405E-81B2-DFF6B78918CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7C15DFF-708F-416D-AB00-CCF5CE9D6635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
     <t>Grade</t>
   </si>
   <si>
-    <t>Issued On</t>
+    <t>IssuedOn</t>
   </si>
   <si>
     <t>Intermediate Python</t>
@@ -1166,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3027,6 +3027,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C797B8AD90D44498DEE196080AFE3F2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d8a7b83c41275397db5e03f2b73eca8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fefa867-d15f-4a0d-9945-ea6297accf67" xmlns:ns3="fadb6cc6-1edc-4022-b9cc-b0c463f8d195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fb96d3b9dc267ba3c8d7f8af4b53bea" ns2:_="" ns3:_="">
     <xsd:import namespace="0fefa867-d15f-4a0d-9945-ea6297accf67"/>
@@ -3243,29 +3258,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
 </file>
</xml_diff>

<commit_message>
Making Experience Details dynamic
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7C15DFF-708F-416D-AB00-CCF5CE9D6635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C359FFDF-A3B9-4A5F-96BF-1D6855525F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certifications" sheetId="1" r:id="rId1"/>
+    <sheet name="Experience" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Certifications!$A$1:$G$52</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="249">
   <si>
     <t>Title</t>
   </si>
@@ -52,6 +53,18 @@
     <t>IssuedOn</t>
   </si>
   <si>
+    <t>Microsoft Certified: Azure Fundamentals</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>H953-9167</t>
+  </si>
+  <si>
+    <t>https://www.credly.com/badges/aa538cc2-e9ed-4416-93be-b2daee06f072</t>
+  </si>
+  <si>
     <t>Intermediate Python</t>
   </si>
   <si>
@@ -82,10 +95,7 @@
     <t>https://www.sololearn.com/certificates/course/en/6923943/1161/landscape/png</t>
   </si>
   <si>
-    <t>Microsoft Certified: Azure Fundamentals</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
+    <t>Microsoft Certified: Azure Data Fundamentals</t>
   </si>
   <si>
     <t>H918-4797</t>
@@ -680,6 +690,93 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/0ByTpvKuPcyWeNlhlZlJqbDNRQ3dueTRlVVN5bHRtUjl0aE53/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>DateFrom</t>
+  </si>
+  <si>
+    <t>DateTo</t>
+  </si>
+  <si>
+    <t>UB Technology Innovations</t>
+  </si>
+  <si>
+    <t>Internship Trainee</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Software Engineer Trainee</t>
+  </si>
+  <si>
+    <t>PRESENT</t>
+  </si>
+  <si>
+    <t>Piblitz</t>
+  </si>
+  <si>
+    <t>Django Developer</t>
+  </si>
+  <si>
+    <t>I have worked on simple and complex tasks in which I gained a lot of knowledge and communication skills. They gave me all kinds of tasks like backend and also front end, before getting into work I thought that JavaScript is not necessary when we work on Django Framework, then after getting into work I realized that JavaScript is necessary for developing Interactive Websites. It was an amazing journey.</t>
+  </si>
+  <si>
+    <t>https://github.com/jjnanthakumar/Certificates-softcopy/blob/main/Piblitz%20Intern%20cert.pdf</t>
+  </si>
+  <si>
+    <t>Tech Nerds</t>
+  </si>
+  <si>
+    <t>Campus Ambassador</t>
+  </si>
+  <si>
+    <t>Learned digital and social media marketing.</t>
+  </si>
+  <si>
+    <t>https://github.com/jjnanthakumar/Certificates-softcopy/blob/main/Tech%20Nerds%20CA.pdf</t>
+  </si>
+  <si>
+    <t>COLCO</t>
+  </si>
+  <si>
+    <t>https://github.com/jjnanthakumar/Certificates-softcopy/blob/main/Campus%20Ambassador%20Intern%20COLCO.pdf</t>
+  </si>
+  <si>
+    <t>Networkz System</t>
+  </si>
+  <si>
+    <t>Intern</t>
+  </si>
+  <si>
+    <t>Got an Wonderful Experience in Networkz System. In that company I worked on some mini projects using Arduino(Robotics)</t>
+  </si>
+  <si>
+    <t>Madurai</t>
+  </si>
+  <si>
+    <t>https://github.com/jjnanthakumar/Certificates-softcopy/blob/main/networkz%20system%20intern.pdf</t>
   </si>
 </sst>
 </file>
@@ -739,7 +836,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -812,12 +909,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -849,6 +959,40 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1164,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1221,10 +1365,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="7">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="G2" s="20">
-        <v>44419</v>
+        <v>44439</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1232,56 +1376,56 @@
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
       </c>
       <c r="G3" s="20">
-        <v>44418</v>
+        <v>44419</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="E4" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21">
         <v>44418</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>19</v>
@@ -1290,10 +1434,10 @@
         <v>20</v>
       </c>
       <c r="F5" s="7">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="G5" s="20">
-        <v>44412</v>
+        <v>44418</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1306,17 +1450,17 @@
       <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="20">
-        <v>44388</v>
+      <c r="F6" s="41">
+        <v>0.88</v>
+      </c>
+      <c r="G6" s="31">
+        <v>44412</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1324,70 +1468,69 @@
         <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="G7" s="20">
-        <v>44348</v>
+        <v>44388</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D8)</f>
-        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
-      </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="20">
-        <v>44346</v>
+        <v>44348</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="6" t="str">
-        <f t="shared" ref="E9:E10" si="0">HYPERLINK("https://ude.my/"&amp; D9)</f>
-        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D9)</f>
+        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="G9" s="20">
-        <v>44339</v>
+        <v>44346</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1398,20 +1541,20 @@
         <v>36</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D10)</f>
+        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
       </c>
       <c r="F10" s="7">
         <v>1</v>
       </c>
       <c r="G10" s="20">
-        <v>44332</v>
+        <v>44339</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1422,37 +1565,37 @@
         <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>41</v>
+      <c r="E11" s="6" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D11)</f>
+        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
       </c>
       <c r="G11" s="20">
-        <v>44312</v>
+        <v>44332</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="6" t="str">
-        <f t="shared" ref="E12:E15" si="1">HYPERLINK("https://ude.my/"&amp; D12)</f>
-        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
+      <c r="E12" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
@@ -1463,26 +1606,26 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D13)</f>
+        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
       </c>
       <c r="F13" s="7">
         <v>1</v>
       </c>
       <c r="G13" s="20">
-        <v>44309</v>
+        <v>44312</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1493,20 +1636,20 @@
         <v>48</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>https://ude.my/UC-1f46a0d1-37f4-4a8c-95f6-839311438ab7</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D14)</f>
+        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
       </c>
       <c r="G14" s="20">
-        <v>44306</v>
+        <v>44309</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1517,20 +1660,20 @@
         <v>51</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E15" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D15)</f>
+        <v>https://ude.my/UC-1f46a0d1-37f4-4a8c-95f6-839311438ab7</v>
       </c>
       <c r="F15" s="13">
         <v>1</v>
       </c>
       <c r="G15" s="21">
-        <v>44300</v>
+        <v>44306</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1541,30 +1684,31 @@
         <v>54</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>56</v>
+      <c r="E16" s="6" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D16)</f>
+        <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
       </c>
       <c r="F16" s="7">
         <v>1</v>
       </c>
       <c r="G16" s="20">
-        <v>44288</v>
+        <v>44300</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>58</v>
@@ -1584,10 +1728,10 @@
         <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>61</v>
@@ -1607,10 +1751,10 @@
         <v>63</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>64</v>
@@ -1622,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="20">
-        <v>44287</v>
+        <v>44288</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1630,10 +1774,10 @@
         <v>66</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>67</v>
@@ -1653,10 +1797,10 @@
         <v>69</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>70</v>
@@ -1676,10 +1820,10 @@
         <v>72</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>73</v>
@@ -1691,7 +1835,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="21">
-        <v>44268</v>
+        <v>44287</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1699,23 +1843,22 @@
         <v>75</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D23)</f>
-        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
-      </c>
       <c r="F23" s="13">
         <v>1</v>
       </c>
       <c r="G23" s="21">
-        <v>44249</v>
+        <v>44268</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1726,30 +1869,31 @@
         <v>79</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>81</v>
+      <c r="E24" s="6" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D24)</f>
+        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
       </c>
       <c r="F24" s="7">
-        <v>0.97</v>
-      </c>
-      <c r="G24" s="19">
-        <v>44246</v>
+        <v>1</v>
+      </c>
+      <c r="G24" s="21">
+        <v>44249</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>54</v>
-      </c>
       <c r="C25" s="12" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>83</v>
@@ -1758,10 +1902,10 @@
         <v>84</v>
       </c>
       <c r="F25" s="7">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G25" s="19">
-        <v>44209</v>
+        <v>44246</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1769,10 +1913,10 @@
         <v>85</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>86</v>
@@ -1784,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="19">
-        <v>44180</v>
+        <v>44209</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1792,92 +1936,92 @@
         <v>88</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="E27" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="8">
-        <v>271676</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="F27" s="13">
         <v>1</v>
       </c>
       <c r="G27" s="19">
-        <v>44176</v>
+        <v>44180</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D28" s="8">
         <v>271676</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F28" s="13">
         <v>1</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="19">
         <v>44176</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C29" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="42">
+        <v>271676</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D29)</f>
-        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
-      </c>
       <c r="F29" s="13">
         <v>1</v>
       </c>
-      <c r="G29" s="17">
-        <v>44165</v>
+      <c r="G29" s="20">
+        <v>44176</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="C30" s="5" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" s="6" t="s">
         <v>98</v>
       </c>
+      <c r="E30" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D30)</f>
+        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
+      </c>
       <c r="F30" s="7">
         <v>1</v>
       </c>
       <c r="G30" s="17">
-        <v>44146</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1885,23 +2029,22 @@
         <v>99</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D31)</f>
-        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
-      </c>
       <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="G31" s="17">
-        <v>44135</v>
+        <v>44146</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1912,13 +2055,14 @@
         <v>103</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>106</v>
+      <c r="E32" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D32)</f>
+        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
       </c>
       <c r="F32" s="7">
         <v>1</v>
@@ -1929,44 +2073,43 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D33)</f>
-        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
+      <c r="E33" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
       <c r="G33" s="17">
-        <v>44126</v>
+        <v>44135</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E34" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D34)</f>
-        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
+        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
@@ -1977,20 +2120,20 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D35)</f>
-        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D35)</f>
+        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
       </c>
       <c r="F35" s="13">
         <v>1</v>
@@ -2001,26 +2144,26 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D36)</f>
-        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D36)</f>
+        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
       </c>
       <c r="F36" s="7">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G36" s="19">
-        <v>44124</v>
+        <v>44126</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2028,20 +2171,20 @@
         <v>116</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E37" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D37)</f>
-        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D37)</f>
+        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
       </c>
       <c r="F37" s="7">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G37" s="19">
         <v>44124</v>
@@ -2049,47 +2192,47 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E38" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D38)</f>
-        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D38)</f>
+        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
       </c>
       <c r="F38" s="7">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G38" s="19">
-        <v>44122</v>
+        <v>44124</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>122</v>
       </c>
       <c r="E39" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D39)</f>
-        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D39)</f>
+        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
       </c>
       <c r="F39" s="7">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G39" s="19">
         <v>44122</v>
@@ -2103,20 +2246,20 @@
         <v>124</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>125</v>
       </c>
       <c r="E40" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D40)</f>
-        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D40)</f>
+        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
       </c>
       <c r="G40" s="19">
-        <v>44112</v>
+        <v>44122</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2124,41 +2267,41 @@
         <v>126</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E41" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D41)</f>
-        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
+        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
       </c>
       <c r="G41" s="19">
-        <v>44105</v>
+        <v>44112</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E42" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D42)</f>
-        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
+        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
       </c>
       <c r="F42" s="16">
         <v>1</v>
@@ -2169,44 +2312,44 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E43" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D43)</f>
-        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
+        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
       </c>
       <c r="F43" s="16">
         <v>1</v>
       </c>
       <c r="G43" s="19">
-        <v>44104</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>131</v>
+        <v>15</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E44" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D44)</f>
-        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
+        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
       </c>
       <c r="F44" s="16">
         <v>1</v>
@@ -2217,90 +2360,91 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>94</v>
+        <v>124</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E45" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D45)</f>
-        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
+        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
       </c>
       <c r="F45" s="16">
         <v>1</v>
       </c>
       <c r="G45" s="19">
-        <v>44080</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>94</v>
+        <v>103</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E46" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D46)</f>
-        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
+        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
       </c>
       <c r="F46" s="16">
         <v>1</v>
       </c>
-      <c r="G46" s="21">
-        <v>44067</v>
+      <c r="G46" s="19">
+        <v>44080</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D47" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>140</v>
+      <c r="E47" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D47)</f>
+        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
       </c>
       <c r="F47" s="16">
         <v>1</v>
       </c>
       <c r="G47" s="21">
-        <v>44066</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>138</v>
-      </c>
       <c r="C48" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F48" s="16">
         <v>1</v>
@@ -2311,19 +2455,19 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
@@ -2334,44 +2478,43 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D50" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E50" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D50)</f>
-        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
+      <c r="B50" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
       </c>
-      <c r="G50" s="17">
-        <v>44063</v>
+      <c r="G50" s="20">
+        <v>44066</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E51" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D51)</f>
-        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D51)</f>
+        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
       </c>
       <c r="F51" s="7">
         <v>1</v>
@@ -2382,169 +2525,170 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>114</v>
+        <v>150</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E52" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D52)</f>
-        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D52)</f>
+        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
       </c>
       <c r="F52" s="13">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G52" s="19">
-        <v>44056</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E53" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D53)</f>
-        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
+        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
       </c>
       <c r="F53" s="7">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="G53" s="17">
-        <v>44055</v>
+        <v>44056</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
-        <v>21</v>
+        <v>154</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>30</v>
+        <v>117</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="E54" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D54)</f>
-        <v>https://ude.my/UC-57e2fe2c-3570-4bb3-862f-19b05a9b4413</v>
+        <v>155</v>
+      </c>
+      <c r="E54" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D54)</f>
+        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
       </c>
       <c r="F54" s="13">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="G54" s="17">
-        <v>44054</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>94</v>
+        <v>24</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E55" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D55)</f>
-        <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
+        <v>156</v>
+      </c>
+      <c r="E55" s="6" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D55)</f>
+        <v>https://ude.my/UC-57e2fe2c-3570-4bb3-862f-19b05a9b4413</v>
       </c>
       <c r="F55" s="13">
         <v>1</v>
       </c>
       <c r="G55" s="17">
-        <v>44022</v>
+        <v>44054</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E56" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D56)</f>
-        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+        <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
       </c>
       <c r="F56" s="13">
         <v>1</v>
       </c>
       <c r="G56" s="17">
-        <v>44021</v>
+        <v>44022</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E57" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D57)</f>
+        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+      </c>
+      <c r="F57" s="13">
+        <v>1</v>
+      </c>
+      <c r="G57" s="17">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E58" s="10" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D58)</f>
         <v>https://www.coursera.org/verify/L4NCNJMVFQPU</v>
       </c>
-      <c r="F57" s="13">
-        <v>1</v>
-      </c>
-      <c r="G57" s="17">
+      <c r="F58" s="13">
+        <v>1</v>
+      </c>
+      <c r="G58" s="19">
         <v>44013</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="F58" s="11">
-        <v>1</v>
-      </c>
-      <c r="G58" s="19">
-        <v>44004</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2552,10 +2696,10 @@
         <v>163</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>164</v>
@@ -2567,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="19">
-        <v>44003</v>
+        <v>44004</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2575,10 +2719,10 @@
         <v>166</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>167</v>
@@ -2594,75 +2738,74 @@
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="5" t="s">
-        <v>11</v>
+      <c r="A61" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E61" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D61)</f>
-        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
-      </c>
-      <c r="F61" s="13">
+        <v>57</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F61" s="11">
         <v>1</v>
       </c>
       <c r="G61" s="19">
-        <v>43999</v>
+        <v>44003</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>94</v>
+        <v>15</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E62" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D62)</f>
-        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
+        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
       </c>
       <c r="F62" s="13">
-        <v>0.94</v>
+        <v>1</v>
       </c>
       <c r="G62" s="19">
-        <v>43995</v>
+        <v>43999</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E63" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D63)</f>
-        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
       </c>
       <c r="F63" s="13">
         <v>0.94</v>
       </c>
       <c r="G63" s="17">
-        <v>43987</v>
+        <v>43995</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2670,46 +2813,47 @@
         <v>175</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>121</v>
+        <v>176</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E64" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D64)</f>
+        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+      </c>
+      <c r="F64" s="13">
+        <v>0.94</v>
+      </c>
+      <c r="G64" s="17">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="E65" s="10" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D65)</f>
         <v>https://www.coursera.org/verify/3W45QQBKACKZ</v>
       </c>
-      <c r="F64" s="13">
-        <v>1</v>
-      </c>
-      <c r="G64" s="17">
+      <c r="F65" s="13">
+        <v>1</v>
+      </c>
+      <c r="G65" s="19">
         <v>43986</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="F65" s="11">
-        <v>1</v>
-      </c>
-      <c r="G65" s="19">
-        <v>43984</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -2717,33 +2861,33 @@
         <v>180</v>
       </c>
       <c r="B66" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="E66" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>184</v>
-      </c>
       <c r="F66" s="11">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G66" s="19">
-        <v>43983</v>
+        <v>43984</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>182</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>186</v>
@@ -2752,105 +2896,105 @@
         <v>187</v>
       </c>
       <c r="F67" s="11">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G67" s="19">
         <v>43983</v>
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C68" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D68" s="5" t="s">
+      <c r="E68" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E68" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D68)</f>
-        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
-      </c>
-      <c r="F68" s="13">
-        <v>0.83</v>
+      <c r="F68" s="11">
+        <v>0.8</v>
       </c>
       <c r="G68" s="17">
         <v>43983</v>
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D69" s="2" t="s">
+      <c r="B69" s="5" t="s">
         <v>192</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="E69" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D69)</f>
-        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
-      </c>
-      <c r="F69" s="11">
-        <v>1</v>
+        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
+      </c>
+      <c r="F69" s="13">
+        <v>0.83</v>
       </c>
       <c r="G69" s="17">
-        <v>43978</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E70" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D70)</f>
-        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
+        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
       </c>
       <c r="F70" s="24">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G70" s="17">
-        <v>43968</v>
+        <v>43978</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E71" s="3" t="s">
         <v>197</v>
       </c>
+      <c r="E71" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D71)</f>
+        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
+      </c>
       <c r="F71" s="24">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G71" s="17">
-        <v>43965</v>
+        <v>43968</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2858,56 +3002,56 @@
         <v>198</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="F72" s="4">
         <v>1</v>
       </c>
       <c r="G72" s="17">
-        <v>43956</v>
+        <v>43965</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="E73" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="F73" s="4">
         <v>1</v>
       </c>
       <c r="G73" s="17">
-        <v>43953</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>208</v>
@@ -2919,7 +3063,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="17">
-        <v>43871</v>
+        <v>43953</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2927,10 +3071,10 @@
         <v>210</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>211</v>
@@ -2942,7 +3086,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="19">
-        <v>43551</v>
+        <v>43871</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2950,98 +3094,377 @@
         <v>213</v>
       </c>
       <c r="B76" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D76" s="2" t="s">
+      <c r="E76" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="F76" s="11">
+        <v>1</v>
+      </c>
+      <c r="G76" s="19">
+        <v>43551</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F76" s="4">
-        <v>1</v>
-      </c>
-      <c r="G76" s="17">
+      <c r="B77" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F77" s="4">
+        <v>1</v>
+      </c>
+      <c r="G77" s="17">
         <v>43549</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G76" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G76">
-      <sortCondition descending="1" ref="G1:G75"/>
+  <autoFilter ref="A1:G77" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G77">
+      <sortCondition descending="1" ref="G1:G77"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E76" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
-    <hyperlink ref="E75" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
-    <hyperlink ref="E74" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
-    <hyperlink ref="E72" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
-    <hyperlink ref="E73" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
-    <hyperlink ref="E70" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
-    <hyperlink ref="E71" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
-    <hyperlink ref="E65" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
-    <hyperlink ref="E66" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
-    <hyperlink ref="E67" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
-    <hyperlink ref="E59" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
-    <hyperlink ref="E60" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
-    <hyperlink ref="E58" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
-    <hyperlink ref="E32" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
-    <hyperlink ref="E30" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
-    <hyperlink ref="E27" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
-    <hyperlink ref="E26" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
-    <hyperlink ref="E25" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
-    <hyperlink ref="E24" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
-    <hyperlink ref="E6" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
-    <hyperlink ref="E3" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
-    <hyperlink ref="E4" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
-    <hyperlink ref="E5" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
-    <hyperlink ref="E7" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
-    <hyperlink ref="E11" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
-    <hyperlink ref="E16" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
-    <hyperlink ref="E19" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
-    <hyperlink ref="E20" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
-    <hyperlink ref="E21" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
-    <hyperlink ref="E17" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
-    <hyperlink ref="E18" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
-    <hyperlink ref="E22" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
-    <hyperlink ref="E28" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
-    <hyperlink ref="E47" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
-    <hyperlink ref="E48" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
-    <hyperlink ref="E49" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
-    <hyperlink ref="E2" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
-    <hyperlink ref="E69" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
+    <hyperlink ref="E77" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
+    <hyperlink ref="E76" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
+    <hyperlink ref="E75" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
+    <hyperlink ref="E73" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
+    <hyperlink ref="E74" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
+    <hyperlink ref="E71" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
+    <hyperlink ref="E72" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
+    <hyperlink ref="E66" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
+    <hyperlink ref="E67" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
+    <hyperlink ref="E68" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
+    <hyperlink ref="E60" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
+    <hyperlink ref="E61" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
+    <hyperlink ref="E59" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
+    <hyperlink ref="E33" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
+    <hyperlink ref="E31" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
+    <hyperlink ref="E28" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
+    <hyperlink ref="E27" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
+    <hyperlink ref="E26" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
+    <hyperlink ref="E25" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
+    <hyperlink ref="E7" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
+    <hyperlink ref="E4" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
+    <hyperlink ref="E5" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
+    <hyperlink ref="E6" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
+    <hyperlink ref="E8" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
+    <hyperlink ref="E12" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
+    <hyperlink ref="E17" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
+    <hyperlink ref="E20" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
+    <hyperlink ref="E21" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
+    <hyperlink ref="E22" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
+    <hyperlink ref="E18" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
+    <hyperlink ref="E19" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
+    <hyperlink ref="E23" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
+    <hyperlink ref="E29" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
+    <hyperlink ref="E48" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
+    <hyperlink ref="E49" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
+    <hyperlink ref="E50" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
+    <hyperlink ref="E3" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
+    <hyperlink ref="E70" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
     <hyperlink ref="E29:E42" r:id="rId39" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{CE0B26B0-E940-4BD5-8F74-8D28A4F3B13A}"/>
-    <hyperlink ref="E29" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
-    <hyperlink ref="E46" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
-    <hyperlink ref="E8" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
+    <hyperlink ref="E30" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
+    <hyperlink ref="E47" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
+    <hyperlink ref="E9" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
     <hyperlink ref="E9:E10" r:id="rId43" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{C55AB7BE-0BE1-4CE1-8CFE-C0E7B2B0BA28}"/>
     <hyperlink ref="E12:E15" r:id="rId44" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{549C4CBA-43AF-4870-BE36-8D1CBC3CFD71}"/>
-    <hyperlink ref="E23" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
-    <hyperlink ref="E54" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
+    <hyperlink ref="E24" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
+    <hyperlink ref="E55" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
+    <hyperlink ref="E2" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7494C2C-9786-4889-8081-3FC41A1A3B3E}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="112.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="107.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" s="31">
+        <v>44263</v>
+      </c>
+      <c r="G2" s="31">
+        <v>44377</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="20">
+        <v>44378</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" s="37" customFormat="1" ht="75">
+      <c r="A4" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="35">
+        <v>44137</v>
+      </c>
+      <c r="G4" s="35">
+        <v>44200</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="F5" s="20">
+        <v>44136</v>
+      </c>
+      <c r="G5" s="20">
+        <v>44166</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="F6" s="20">
+        <v>44105</v>
+      </c>
+      <c r="G6" s="20">
+        <v>44136</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" s="20">
+        <v>43432</v>
+      </c>
+      <c r="G7" s="20">
+        <v>43442</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{F023270F-32A2-4084-BC0C-759F75126131}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{36657B35-2DE3-4353-875D-05EDE8EC8328}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{424F7718-10F0-4367-9C1C-C1FF49F2EBFA}"/>
+    <hyperlink ref="I7" r:id="rId4" xr:uid="{004196DD-DF68-41F8-8E08-7FF73A789B6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C797B8AD90D44498DEE196080AFE3F2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d8a7b83c41275397db5e03f2b73eca8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fefa867-d15f-4a0d-9945-ea6297accf67" xmlns:ns3="fadb6cc6-1edc-4022-b9cc-b0c463f8d195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fb96d3b9dc267ba3c8d7f8af4b53bea" ns2:_="" ns3:_="">
     <xsd:import namespace="0fefa867-d15f-4a0d-9945-ea6297accf67"/>
@@ -3258,14 +3681,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
 </file>
</xml_diff>

<commit_message>
Fixed Experience Section with Dynamic Data
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C359FFDF-A3B9-4A5F-96BF-1D6855525F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3265A74-381B-490C-890A-685F08814246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certifications" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Certifications!$A$1:$G$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Experience!$A$1:$I$7</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="251">
   <si>
     <t>Title</t>
   </si>
@@ -716,22 +717,28 @@
     <t>UB Technology Innovations</t>
   </si>
   <si>
+    <t>Software Engineer Trainee</t>
+  </si>
+  <si>
+    <t>Currently Working on Analytics in a Day Event and Hackathon Solution.</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>PRESENT</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>Internship Trainee</t>
   </si>
   <si>
-    <t>Remote</t>
+    <t>Worked on Azure Synapse Hackathon and implemented Devops for Azure Synapse.</t>
   </si>
   <si>
     <t>COMPLETED</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Software Engineer Trainee</t>
-  </si>
-  <si>
-    <t>PRESENT</t>
   </si>
   <si>
     <t>Piblitz</t>
@@ -1310,7 +1317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -3198,8 +3205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7494C2C-9786-4889-8081-3FC41A1A3B3E}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3250,21 +3257,23 @@
       <c r="B2" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C2" s="29"/>
+      <c r="C2" s="29" t="s">
+        <v>229</v>
+      </c>
       <c r="D2" s="29" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F2" s="31">
-        <v>44263</v>
-      </c>
-      <c r="G2" s="31">
-        <v>44377</v>
+        <v>44378</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>231</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I2" s="5"/>
     </row>
@@ -3273,41 +3282,43 @@
         <v>227</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="20">
+        <v>44263</v>
+      </c>
+      <c r="G3" s="20">
+        <v>44377</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="F3" s="20">
-        <v>44378</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>231</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" s="37" customFormat="1" ht="75">
       <c r="A4" s="32" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B4" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="34" t="s">
         <v>235</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>230</v>
       </c>
       <c r="F4" s="35">
         <v>44137</v>
@@ -3316,27 +3327,27 @@
         <v>44200</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F5" s="20">
         <v>44136</v>
@@ -3345,27 +3356,27 @@
         <v>44166</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>240</v>
-      </c>
       <c r="D6" s="29" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F6" s="20">
         <v>44105</v>
@@ -3374,27 +3385,27 @@
         <v>44136</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F7" s="20">
         <v>43432</v>
@@ -3403,10 +3414,10 @@
         <v>43442</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3454,6 +3465,11 @@
       <c r="I11" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I7" xr:uid="{B7494C2C-9786-4889-8081-3FC41A1A3B3E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I7">
+      <sortCondition descending="1" ref="F1:F7"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{F023270F-32A2-4084-BC0C-759F75126131}"/>
     <hyperlink ref="I5" r:id="rId2" xr:uid="{36657B35-2DE3-4353-875D-05EDE8EC8328}"/>

</xml_diff>

<commit_message>
Project Contents Updated with Dynamic Content
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24504"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8444BCAD-3A93-4955-BD10-AC38BF8A0243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21497508-36F0-4B1D-84FD-6C281DECC33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certifications" sheetId="1" r:id="rId1"/>
     <sheet name="Experience" sheetId="2" r:id="rId2"/>
     <sheet name="Skills" sheetId="3" r:id="rId3"/>
+    <sheet name="Projects" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Certifications!$A$1:$G$52</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="307">
   <si>
     <t>Title</t>
   </si>
@@ -845,6 +846,114 @@
   </si>
   <si>
     <t>PYQT5</t>
+  </si>
+  <si>
+    <t>ProjectURL</t>
+  </si>
+  <si>
+    <t>CoverImage</t>
+  </si>
+  <si>
+    <t>Blood Bank Data Storage Using User Authentication with OTP APIs (limited access)</t>
+  </si>
+  <si>
+    <t>Web Development</t>
+  </si>
+  <si>
+    <t>https://bloodbk.herokuapp.com</t>
+  </si>
+  <si>
+    <t>images/project-1.jpg</t>
+  </si>
+  <si>
+    <t>Simple Flames Game Site</t>
+  </si>
+  <si>
+    <t>https://nandy-flamesgame.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>images/project-2.jpg</t>
+  </si>
+  <si>
+    <t>Face Detection using OpenCV Python</t>
+  </si>
+  <si>
+    <t>https://nandyfacedetect.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>images/project-3.jpg</t>
+  </si>
+  <si>
+    <t>CRUD Social media app using MERN stack</t>
+  </si>
+  <si>
+    <t>https://mempro.netlify.app</t>
+  </si>
+  <si>
+    <t>images/mem.jpg</t>
+  </si>
+  <si>
+    <t>React Todo App (using localstorage)</t>
+  </si>
+  <si>
+    <t>https://jjnanthakumar.github.io/reacttodo</t>
+  </si>
+  <si>
+    <t>images/todo.jpg</t>
+  </si>
+  <si>
+    <t>Simple Chat App Using chatengine.io [API]</t>
+  </si>
+  <si>
+    <t>https://nandy-chatapp.netlify.app</t>
+  </si>
+  <si>
+    <t>images/chat.jpg</t>
+  </si>
+  <si>
+    <t>imple Weather Progressive Web App Using openweather Map [API]</t>
+  </si>
+  <si>
+    <t>https://nandy-weatherapp.netlify.app</t>
+  </si>
+  <si>
+    <t>images/weather.jpg</t>
+  </si>
+  <si>
+    <t>Simple Recipe Search Web App Using API</t>
+  </si>
+  <si>
+    <t>https://jjnanthakumar.github.io/reactrecipe</t>
+  </si>
+  <si>
+    <t>images/recipe.jpg</t>
+  </si>
+  <si>
+    <t>Covid-19 Tracker Web App Using API</t>
+  </si>
+  <si>
+    <t>https://nandy-covid19.netlify.app/</t>
+  </si>
+  <si>
+    <t>images/covid.jpg</t>
+  </si>
+  <si>
+    <t>Twitter Opinion Mining Web App Using Django</t>
+  </si>
+  <si>
+    <t>https://nlptweets.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>images/twitter.jpg</t>
+  </si>
+  <si>
+    <t>Embedly Web App Using Django</t>
+  </si>
+  <si>
+    <t>https://nandyembedly.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>images/embed.jpg</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1070,6 +1179,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3554,8 +3664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718451B2-E12D-4ABD-B26C-5975AED3964E}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B20" sqref="A20:B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3725,6 +3835,208 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DB9CC9-BE76-4E73-A91C-99466DD45DAE}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6C019AFC-BBAE-44A4-B6C9-EB4D5322203E}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{E0C77B21-62EA-4BB6-A252-BCDBF2A329C9}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{58A5056C-7DF9-41FA-9FE7-199F9656DBAA}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{8C68520D-65C7-4CAE-A74F-DBBCF65440FD}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{B1186454-361F-423A-B104-A0609BD187BF}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{F7227DFD-66E4-484A-BDE9-07BA7E5DE89C}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{CB93CFCA-7A01-4646-87F7-16ABE9BE54E7}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{B90D1A29-BEB8-4132-AFCA-64664123C53E}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{507DFA43-E3D5-43C2-A565-2656041B0BBF}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{509BDAC4-93D8-4C25-91D3-B14897D80AE5}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{C029E0E5-B966-4A9C-8212-4AEC7FF5106B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added Two Certifications - JavaScript(Basic, Intermediate) from HackerRank
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24519"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24617"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B5EF10D-41A6-48B6-AD6A-2743F7399512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D3AA1EB-CF60-48A1-A9FB-845721667557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="304">
   <si>
     <t>Title</t>
   </si>
@@ -672,6 +672,18 @@
   </si>
   <si>
     <t>eafe133d26dc</t>
+  </si>
+  <si>
+    <t>JavaScript (Basic)</t>
+  </si>
+  <si>
+    <t>7a872682b210</t>
+  </si>
+  <si>
+    <t>JavaScript (Intermediate)</t>
+  </si>
+  <si>
+    <t>524e499db551</t>
   </si>
   <si>
     <t>Company</t>
@@ -1123,7 +1135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1202,6 +1214,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1517,11 +1530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1581,7 +1593,7 @@
         <v>44412</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1604,7 +1616,7 @@
         <v>44419</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -1627,7 +1639,7 @@
         <v>44418</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>44439</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -1696,7 +1708,7 @@
         <v>44388</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1719,7 +1731,7 @@
         <v>44348</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1">
+    <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -1743,7 +1755,7 @@
         <v>44346</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1">
+    <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1767,7 +1779,7 @@
         <v>44339</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1">
+    <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -1791,7 +1803,7 @@
         <v>44332</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1">
+    <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -1814,7 +1826,7 @@
         <v>44312</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1">
+    <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
         <v>45</v>
       </c>
@@ -1838,7 +1850,7 @@
         <v>44312</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1">
+    <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -1862,7 +1874,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1">
+    <row r="15" spans="1:7">
       <c r="A15" s="12" t="s">
         <v>50</v>
       </c>
@@ -1886,7 +1898,7 @@
         <v>44306</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1">
+    <row r="16" spans="1:7">
       <c r="A16" s="12" t="s">
         <v>53</v>
       </c>
@@ -1910,7 +1922,7 @@
         <v>44300</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
+    <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
@@ -1934,7 +1946,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
+    <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
         <v>59</v>
       </c>
@@ -1958,7 +1970,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
         <v>61</v>
       </c>
@@ -1982,7 +1994,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
+    <row r="20" spans="1:7">
       <c r="A20" s="28" t="s">
         <v>63</v>
       </c>
@@ -2005,7 +2017,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" spans="1:7">
       <c r="A21" s="12" t="s">
         <v>66</v>
       </c>
@@ -2028,7 +2040,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>69</v>
       </c>
@@ -2051,7 +2063,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
         <v>72</v>
       </c>
@@ -2075,7 +2087,7 @@
         <v>44268</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
+    <row r="24" spans="1:7">
       <c r="A24" s="28" t="s">
         <v>74</v>
       </c>
@@ -2099,7 +2111,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
+    <row r="25" spans="1:7">
       <c r="A25" s="12" t="s">
         <v>77</v>
       </c>
@@ -2122,7 +2134,7 @@
         <v>44246</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
         <v>81</v>
       </c>
@@ -2146,7 +2158,7 @@
         <v>44209</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="28" t="s">
         <v>83</v>
       </c>
@@ -2169,7 +2181,7 @@
         <v>44180</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
+    <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
         <v>86</v>
       </c>
@@ -2192,7 +2204,7 @@
         <v>44176</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="12" t="s">
         <v>86</v>
       </c>
@@ -2215,7 +2227,7 @@
         <v>44176</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="12" t="s">
         <v>90</v>
       </c>
@@ -2239,7 +2251,7 @@
         <v>44165</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
+    <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
         <v>94</v>
       </c>
@@ -2263,7 +2275,7 @@
         <v>44146</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
+    <row r="32" spans="1:7">
       <c r="A32" s="28" t="s">
         <v>96</v>
       </c>
@@ -2287,7 +2299,7 @@
         <v>44135</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>99</v>
       </c>
@@ -2310,7 +2322,7 @@
         <v>44135</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>104</v>
       </c>
@@ -2334,7 +2346,7 @@
         <v>44126</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1">
+    <row r="35" spans="1:7">
       <c r="A35" s="12" t="s">
         <v>106</v>
       </c>
@@ -2358,7 +2370,7 @@
         <v>44126</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>108</v>
       </c>
@@ -2382,7 +2394,7 @@
         <v>44126</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>110</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>44124</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1">
+    <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
         <v>113</v>
       </c>
@@ -2430,7 +2442,7 @@
         <v>44124</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1">
+    <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
         <v>115</v>
       </c>
@@ -2454,7 +2466,7 @@
         <v>44122</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
         <v>117</v>
       </c>
@@ -2478,7 +2490,7 @@
         <v>44122</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1">
+    <row r="41" spans="1:7">
       <c r="A41" s="12" t="s">
         <v>120</v>
       </c>
@@ -2502,7 +2514,7 @@
         <v>44112</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1">
+    <row r="42" spans="1:7">
       <c r="A42" s="12" t="s">
         <v>123</v>
       </c>
@@ -2526,7 +2538,7 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
         <v>125</v>
       </c>
@@ -2550,7 +2562,7 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1">
+    <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
         <v>15</v>
       </c>
@@ -2574,7 +2586,7 @@
         <v>44104</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1">
+    <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -2598,7 +2610,7 @@
         <v>44104</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1">
+    <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
         <v>130</v>
       </c>
@@ -2622,7 +2634,7 @@
         <v>44080</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>132</v>
       </c>
@@ -2646,7 +2658,7 @@
         <v>44067</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>134</v>
       </c>
@@ -2669,7 +2681,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1">
+    <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
         <v>138</v>
       </c>
@@ -2692,7 +2704,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1">
+    <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
         <v>140</v>
       </c>
@@ -2715,7 +2727,7 @@
         <v>44066</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1">
+    <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
         <v>142</v>
       </c>
@@ -2739,7 +2751,7 @@
         <v>44063</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1">
+    <row r="52" spans="1:7">
       <c r="A52" s="12" t="s">
         <v>144</v>
       </c>
@@ -2763,7 +2775,7 @@
         <v>44063</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1">
+    <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
         <v>146</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>44056</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1">
+    <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
         <v>148</v>
       </c>
@@ -2811,7 +2823,7 @@
         <v>44055</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1">
+    <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
         <v>24</v>
       </c>
@@ -2835,7 +2847,7 @@
         <v>44054</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1">
+    <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
         <v>151</v>
       </c>
@@ -2859,7 +2871,7 @@
         <v>44022</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1">
+    <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
         <v>153</v>
       </c>
@@ -2883,7 +2895,7 @@
         <v>44021</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1">
+    <row r="58" spans="1:7">
       <c r="A58" s="12" t="s">
         <v>155</v>
       </c>
@@ -2907,7 +2919,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1">
+    <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
         <v>157</v>
       </c>
@@ -2931,7 +2943,7 @@
         <v>44004</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1">
+    <row r="60" spans="1:7">
       <c r="A60" s="2" t="s">
         <v>159</v>
       </c>
@@ -2955,7 +2967,7 @@
         <v>44003</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1">
+    <row r="61" spans="1:7">
       <c r="A61" s="2" t="s">
         <v>161</v>
       </c>
@@ -2979,7 +2991,7 @@
         <v>44003</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1">
+    <row r="62" spans="1:7">
       <c r="A62" s="28" t="s">
         <v>15</v>
       </c>
@@ -3003,7 +3015,7 @@
         <v>43999</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1">
+    <row r="63" spans="1:7">
       <c r="A63" s="5" t="s">
         <v>164</v>
       </c>
@@ -3027,7 +3039,7 @@
         <v>43995</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1">
+    <row r="64" spans="1:7">
       <c r="A64" s="5" t="s">
         <v>166</v>
       </c>
@@ -3051,7 +3063,7 @@
         <v>43987</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1">
+    <row r="65" spans="1:7">
       <c r="A65" s="12" t="s">
         <v>169</v>
       </c>
@@ -3075,7 +3087,7 @@
         <v>43986</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1">
+    <row r="66" spans="1:7">
       <c r="A66" s="9" t="s">
         <v>171</v>
       </c>
@@ -3098,7 +3110,7 @@
         <v>43984</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1">
+    <row r="67" spans="1:7">
       <c r="A67" s="9" t="s">
         <v>174</v>
       </c>
@@ -3121,7 +3133,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1">
+    <row r="68" spans="1:7">
       <c r="A68" s="2" t="s">
         <v>179</v>
       </c>
@@ -3144,7 +3156,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1">
+    <row r="69" spans="1:7">
       <c r="A69" s="24" t="s">
         <v>182</v>
       </c>
@@ -3168,7 +3180,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1">
+    <row r="70" spans="1:7">
       <c r="A70" s="2" t="s">
         <v>185</v>
       </c>
@@ -3192,7 +3204,7 @@
         <v>43978</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1">
+    <row r="71" spans="1:7">
       <c r="A71" s="2" t="s">
         <v>187</v>
       </c>
@@ -3216,7 +3228,7 @@
         <v>43968</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1">
+    <row r="72" spans="1:7">
       <c r="A72" s="2" t="s">
         <v>189</v>
       </c>
@@ -3239,7 +3251,7 @@
         <v>43965</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1">
+    <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
         <v>192</v>
       </c>
@@ -3262,7 +3274,7 @@
         <v>43956</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1">
+    <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
         <v>196</v>
       </c>
@@ -3285,7 +3297,7 @@
         <v>43953</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1">
+    <row r="75" spans="1:7">
       <c r="A75" s="9" t="s">
         <v>201</v>
       </c>
@@ -3308,7 +3320,7 @@
         <v>43871</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1">
+    <row r="76" spans="1:7">
       <c r="A76" s="2" t="s">
         <v>204</v>
       </c>
@@ -3331,7 +3343,7 @@
         <v>43551</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1">
+    <row r="77" spans="1:7">
       <c r="A77" s="9" t="s">
         <v>207</v>
       </c>
@@ -3354,7 +3366,7 @@
         <v>43549</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1">
+    <row r="78" spans="1:7">
       <c r="A78" s="5" t="s">
         <v>211</v>
       </c>
@@ -3378,13 +3390,56 @@
         <v>44469</v>
       </c>
     </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E79" s="6" t="str">
+        <f t="shared" ref="E79:E80" si="2" xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D79)</f>
+        <v>https://www.hackerrank.com/certificates/7a872682b210</v>
+      </c>
+      <c r="F79" s="7">
+        <v>1</v>
+      </c>
+      <c r="G79" s="20">
+        <v>44490</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D80" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E80" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D80)</f>
+        <v>https://www.hackerrank.com/certificates/524e499db551</v>
+      </c>
+      <c r="F80" s="7">
+        <v>1</v>
+      </c>
+      <c r="G80" s="20">
+        <v>44493</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G78" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Microsoft"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:G80" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G77">
       <sortCondition descending="1" ref="G1:G77"/>
     </sortState>
@@ -3465,25 +3520,25 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>3</v>
@@ -3494,46 +3549,46 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F2" s="30">
         <v>44378</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C3" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>223</v>
-      </c>
       <c r="E3" s="28" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F3" s="20">
         <v>44263</v>
@@ -3542,25 +3597,25 @@
         <v>44377</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" s="36" customFormat="1" ht="75">
       <c r="A4" s="31" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F4" s="34">
         <v>44137</v>
@@ -3569,27 +3624,27 @@
         <v>44200</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F5" s="20">
         <v>44136</v>
@@ -3598,27 +3653,27 @@
         <v>44166</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F6" s="20">
         <v>44105</v>
@@ -3627,27 +3682,27 @@
         <v>44136</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F7" s="20">
         <v>43432</v>
@@ -3656,10 +3711,10 @@
         <v>43442</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3738,15 +3793,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="42" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B2" s="7">
         <v>0.9</v>
@@ -3754,7 +3809,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B3" s="7">
         <v>0.6</v>
@@ -3762,7 +3817,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B4" s="7">
         <v>0.6</v>
@@ -3778,7 +3833,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B6" s="7">
         <v>0.7</v>
@@ -3786,7 +3841,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B7" s="7">
         <v>0.8</v>
@@ -3794,7 +3849,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B8" s="7">
         <v>0.8</v>
@@ -3802,7 +3857,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B9" s="7">
         <v>0.8</v>
@@ -3810,7 +3865,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B10" s="7">
         <v>0.7</v>
@@ -3818,7 +3873,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="12" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B11" s="13">
         <v>0.7</v>
@@ -3826,7 +3881,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="12" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B12" s="13">
         <v>0.8</v>
@@ -3834,7 +3889,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="12" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B13" s="16">
         <v>0.8</v>
@@ -3842,7 +3897,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B14" s="13">
         <v>0.6</v>
@@ -3850,7 +3905,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="12" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B15" s="13">
         <v>0.6</v>
@@ -3858,7 +3913,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="12" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B16" s="13">
         <v>0.6</v>
@@ -3866,7 +3921,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B17" s="7">
         <v>0.5</v>
@@ -3874,7 +3929,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="12" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B18" s="13">
         <v>0.5</v>
@@ -3882,7 +3937,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="12" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B19" s="13">
         <v>0.7</v>
@@ -3890,7 +3945,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B20" s="7">
         <v>0.6</v>
@@ -3906,7 +3961,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3922,167 +3977,167 @@
         <v>0</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="12" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="37" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4104,15 +4159,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C797B8AD90D44498DEE196080AFE3F2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d8a7b83c41275397db5e03f2b73eca8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fefa867-d15f-4a0d-9945-ea6297accf67" xmlns:ns3="fadb6cc6-1edc-4022-b9cc-b0c463f8d195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fb96d3b9dc267ba3c8d7f8af4b53bea" ns2:_="" ns3:_="">
     <xsd:import namespace="0fefa867-d15f-4a0d-9945-ea6297accf67"/>
@@ -4329,20 +4375,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
 </file>
</xml_diff>

<commit_message>
Display order changed from newest to older in excel sheet
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24617"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D3AA1EB-CF60-48A1-A9FB-845721667557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEB3804C-FD35-400B-8838-09F5CE1F95C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,57 +56,78 @@
     <t>IssuedOn</t>
   </si>
   <si>
+    <t>JavaScript (Intermediate)</t>
+  </si>
+  <si>
+    <t>HackerRank</t>
+  </si>
+  <si>
+    <t>524e499db551</t>
+  </si>
+  <si>
+    <t>JavaScript (Basic)</t>
+  </si>
+  <si>
+    <t>7a872682b210</t>
+  </si>
+  <si>
+    <t>Problem Solving (Intermediate)</t>
+  </si>
+  <si>
+    <t>eafe133d26dc</t>
+  </si>
+  <si>
+    <t>Microsoft Certified: Azure Data Fundamentals</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>H918-4797</t>
+  </si>
+  <si>
+    <t>https://www.credly.com/badges/aa538cc2-e9ed-4416-93be-b2daee06f072</t>
+  </si>
+  <si>
+    <t>Intermediate Python</t>
+  </si>
+  <si>
+    <t>SoloLearn</t>
+  </si>
+  <si>
+    <t>6923943-1158</t>
+  </si>
+  <si>
+    <t>https://www.sololearn.com/certificates/course/en/6923943/1158/landscape/png</t>
+  </si>
+  <si>
+    <t>Python Data Structures</t>
+  </si>
+  <si>
+    <t>6923943-1159</t>
+  </si>
+  <si>
+    <t>https://www.sololearn.com/certificates/course/en/6923943/1159/landscape/png</t>
+  </si>
+  <si>
+    <t>Python for Data Science</t>
+  </si>
+  <si>
+    <t>6923943-1161</t>
+  </si>
+  <si>
+    <t>https://www.sololearn.com/certificates/course/en/6923943/1161/landscape/png</t>
+  </si>
+  <si>
     <t>Microsoft Certified: Azure Fundamentals</t>
   </si>
   <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
     <t>H953-9167</t>
   </si>
   <si>
     <t>https://www.credly.com/badges/5b471ed6-57b5-466c-9d5c-654d5f5debca?source=linked_in_profile</t>
   </si>
   <si>
-    <t>Intermediate Python</t>
-  </si>
-  <si>
-    <t>SoloLearn</t>
-  </si>
-  <si>
-    <t>6923943-1158</t>
-  </si>
-  <si>
-    <t>https://www.sololearn.com/certificates/course/en/6923943/1158/landscape/png</t>
-  </si>
-  <si>
-    <t>Python Data Structures</t>
-  </si>
-  <si>
-    <t>6923943-1159</t>
-  </si>
-  <si>
-    <t>https://www.sololearn.com/certificates/course/en/6923943/1159/landscape/png</t>
-  </si>
-  <si>
-    <t>Python for Data Science</t>
-  </si>
-  <si>
-    <t>6923943-1161</t>
-  </si>
-  <si>
-    <t>https://www.sololearn.com/certificates/course/en/6923943/1161/landscape/png</t>
-  </si>
-  <si>
-    <t>Microsoft Certified: Azure Data Fundamentals</t>
-  </si>
-  <si>
-    <t>H918-4797</t>
-  </si>
-  <si>
-    <t>https://www.credly.com/badges/aa538cc2-e9ed-4416-93be-b2daee06f072</t>
-  </si>
-  <si>
     <t>Python for Beginners</t>
   </si>
   <si>
@@ -206,9 +227,6 @@
     <t>Cascading Style Sheet</t>
   </si>
   <si>
-    <t>HackerRank</t>
-  </si>
-  <si>
     <t>cf58231a440f</t>
   </si>
   <si>
@@ -666,24 +684,6 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/0ByTpvKuPcyWeNlhlZlJqbDNRQ3dueTRlVVN5bHRtUjl0aE53/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>Problem Solving (Intermediate)</t>
-  </si>
-  <si>
-    <t>eafe133d26dc</t>
-  </si>
-  <si>
-    <t>JavaScript (Basic)</t>
-  </si>
-  <si>
-    <t>7a872682b210</t>
-  </si>
-  <si>
-    <t>JavaScript (Intermediate)</t>
-  </si>
-  <si>
-    <t>524e499db551</t>
   </si>
   <si>
     <t>Company</t>
@@ -1135,7 +1135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1212,9 +1212,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1532,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1574,424 +1576,424 @@
       <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="39" t="s">
-        <v>10</v>
+      <c r="E2" s="39" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D2)</f>
+        <v>https://www.hackerrank.com/certificates/524e499db551</v>
       </c>
       <c r="F2" s="40">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="G2" s="30">
-        <v>44412</v>
+        <v>44493</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
+      <c r="E3" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D3)</f>
+        <v>https://www.hackerrank.com/certificates/7a872682b210</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
       </c>
       <c r="G3" s="20">
-        <v>44419</v>
+        <v>44490</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="38" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D4)</f>
+        <v>https://www.hackerrank.com/certificates/eafe133d26dc</v>
       </c>
       <c r="F4" s="13">
         <v>1</v>
       </c>
       <c r="G4" s="21">
-        <v>44418</v>
+        <v>44469</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F5" s="7">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="G5" s="20">
-        <v>44418</v>
+        <v>44439</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" s="40">
-        <v>0.94</v>
+        <v>1</v>
       </c>
       <c r="G6" s="30">
-        <v>44439</v>
+        <v>44419</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="G7" s="20">
-        <v>44388</v>
+        <v>44418</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="7">
         <v>1</v>
       </c>
       <c r="G8" s="20">
-        <v>44348</v>
+        <v>44418</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D9)</f>
-        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="F9" s="7">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="G9" s="20">
-        <v>44346</v>
+        <v>44412</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D10)</f>
-        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
-      </c>
       <c r="F10" s="7">
         <v>1</v>
       </c>
       <c r="G10" s="20">
-        <v>44339</v>
+        <v>44388</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D11)</f>
-        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
+        <v>36</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
       </c>
       <c r="G11" s="20">
-        <v>44332</v>
+        <v>44348</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>44</v>
+      <c r="E12" s="6" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D12)</f>
+        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
       </c>
       <c r="G12" s="20">
-        <v>44312</v>
+        <v>44346</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E13" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D13)</f>
-        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
+        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
       </c>
       <c r="F13" s="7">
         <v>1</v>
       </c>
       <c r="G13" s="20">
-        <v>44312</v>
+        <v>44339</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D14)</f>
-        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
+        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
       </c>
       <c r="G14" s="20">
-        <v>44309</v>
+        <v>44332</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="E15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D15)</f>
-        <v>https://ude.my/UC-1f46a0d1-37f4-4a8c-95f6-839311438ab7</v>
-      </c>
       <c r="F15" s="13">
         <v>1</v>
       </c>
       <c r="G15" s="21">
-        <v>44306</v>
+        <v>44312</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="E16" s="38" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D16)</f>
-        <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
+        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
       </c>
       <c r="F16" s="13">
         <v>1</v>
       </c>
       <c r="G16" s="21">
-        <v>44300</v>
+        <v>44312</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="E17" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D17)</f>
-        <v>https://www.hackerrank.com/certificates/cf58231a440f</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D17)</f>
+        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
       </c>
       <c r="F17" s="7">
         <v>1</v>
       </c>
       <c r="G17" s="20">
-        <v>44288</v>
+        <v>44309</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E18" s="6" t="str">
-        <f t="shared" ref="E18:E19" si="0" xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D18)</f>
-        <v>https://www.hackerrank.com/certificates/4490b4a0e606</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D18)</f>
+        <v>https://ude.my/UC-1f46a0d1-37f4-4a8c-95f6-839311438ab7</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="G18" s="20">
-        <v>44288</v>
+        <v>44306</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="C19" s="5" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>https://www.hackerrank.com/certificates/fdeeaad81310</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D19)</f>
+        <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
       </c>
       <c r="G19" s="20">
-        <v>44288</v>
+        <v>44300</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1999,399 +2001,399 @@
         <v>63</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="39" t="s">
-        <v>65</v>
+      <c r="E20" s="39" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D20)</f>
+        <v>https://www.hackerrank.com/certificates/cf58231a440f</v>
       </c>
       <c r="F20" s="40">
         <v>1</v>
       </c>
       <c r="G20" s="30">
-        <v>44287</v>
+        <v>44288</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>68</v>
+      <c r="E21" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D21)</f>
+        <v>https://www.hackerrank.com/certificates/4490b4a0e606</v>
       </c>
       <c r="F21" s="13">
         <v>1</v>
       </c>
       <c r="G21" s="21">
-        <v>44287</v>
+        <v>44288</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="E22" s="38" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D22)</f>
+        <v>https://www.hackerrank.com/certificates/fdeeaad81310</v>
       </c>
       <c r="F22" s="13">
         <v>1</v>
       </c>
       <c r="G22" s="21">
-        <v>44287</v>
+        <v>44288</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D23)</f>
-        <v>https://www.hackerrank.com/certificates/1cadc360a79d</v>
+        <v>70</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
       </c>
       <c r="G23" s="20">
-        <v>44268</v>
+        <v>44287</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="39" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D24)</f>
-        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
-      </c>
       <c r="F24" s="40">
         <v>1</v>
       </c>
       <c r="G24" s="48">
-        <v>44249</v>
+        <v>44287</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>80</v>
-      </c>
       <c r="F25" s="13">
-        <v>0.97</v>
-      </c>
-      <c r="G25" s="19">
-        <v>44246</v>
+        <v>1</v>
+      </c>
+      <c r="G25" s="21">
+        <v>44287</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E26" s="6" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D26)</f>
-        <v>https://www.hackerrank.com/certificates/6730CF1D0F21</v>
+        <v>https://www.hackerrank.com/certificates/1cadc360a79d</v>
       </c>
       <c r="F26" s="7">
         <v>1</v>
       </c>
-      <c r="G26" s="17">
-        <v>44209</v>
+      <c r="G26" s="20">
+        <v>44268</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B27" s="47" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="E27" s="39" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D27)</f>
+        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
       </c>
       <c r="F27" s="49">
         <v>1</v>
       </c>
-      <c r="G27" s="50">
-        <v>44180</v>
+      <c r="G27" s="48">
+        <v>44249</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="8">
-        <v>271676</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>89</v>
-      </c>
       <c r="F28" s="13">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G28" s="19">
-        <v>44176</v>
+        <v>44246</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="41">
-        <v>271676</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>89</v>
+      <c r="E29" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D29)</f>
+        <v>https://www.hackerrank.com/certificates/6730CF1D0F21</v>
       </c>
       <c r="F29" s="13">
         <v>1</v>
       </c>
-      <c r="G29" s="20">
-        <v>44176</v>
+      <c r="G29" s="17">
+        <v>44209</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="E30" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D30)</f>
-        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
-      </c>
       <c r="F30" s="13">
         <v>1</v>
       </c>
       <c r="G30" s="19">
-        <v>44165</v>
+        <v>44180</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="8">
+        <v>271676</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D31)</f>
-        <v>https://www.hackerrank.com/certificates/3AF4DDB28FAB</v>
-      </c>
       <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="G31" s="17">
-        <v>44146</v>
+        <v>44176</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="51" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D32)</f>
-        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
+        <v>94</v>
+      </c>
+      <c r="D32" s="55">
+        <v>271676</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>95</v>
       </c>
       <c r="F32" s="40">
         <v>1</v>
       </c>
-      <c r="G32" s="52">
-        <v>44135</v>
+      <c r="G32" s="30">
+        <v>44176</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>103</v>
+      <c r="E33" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D33)</f>
+        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
       <c r="G33" s="17">
-        <v>44135</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E34" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D34)</f>
-        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
+        <v>101</v>
+      </c>
+      <c r="E34" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D34)</f>
+        <v>https://www.hackerrank.com/certificates/3AF4DDB28FAB</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
       <c r="G34" s="17">
-        <v>44126</v>
+        <v>44146</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E35" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D35)</f>
-        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
+        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
       </c>
       <c r="F35" s="13">
         <v>1</v>
       </c>
       <c r="G35" s="19">
-        <v>44126</v>
+        <v>44135</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D36)</f>
-        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
-      </c>
       <c r="F36" s="7">
         <v>1</v>
       </c>
       <c r="G36" s="19">
-        <v>44126</v>
+        <v>44135</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2399,263 +2401,263 @@
         <v>110</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E37" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D37)</f>
-        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
+        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
       </c>
       <c r="F37" s="7">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G37" s="19">
-        <v>44124</v>
+        <v>44126</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="E38" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D38)</f>
-        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D38)</f>
+        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
       </c>
       <c r="G38" s="19">
-        <v>44124</v>
+        <v>44126</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="E39" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D39)</f>
-        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D39)</f>
+        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
       </c>
       <c r="F39" s="7">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G39" s="19">
-        <v>44122</v>
+        <v>44126</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="E40" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D40)</f>
-        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D40)</f>
+        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
       </c>
       <c r="F40" s="7">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G40" s="19">
-        <v>44122</v>
+        <v>44124</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="E41" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D41)</f>
-        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D41)</f>
+        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
       </c>
       <c r="G41" s="19">
-        <v>44112</v>
+        <v>44124</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E42" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D42)</f>
-        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
+        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
       </c>
       <c r="F42" s="16">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G42" s="19">
-        <v>44105</v>
+        <v>44122</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="E43" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D43)</f>
-        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D43)</f>
+        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
       </c>
       <c r="F43" s="16">
         <v>1</v>
       </c>
       <c r="G43" s="19">
-        <v>44105</v>
+        <v>44122</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E44" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D44)</f>
-        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
+        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
       </c>
       <c r="F44" s="16">
         <v>1</v>
       </c>
       <c r="G44" s="19">
-        <v>44104</v>
+        <v>44112</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E45" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D45)</f>
-        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
+        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
       </c>
       <c r="F45" s="16">
         <v>1</v>
       </c>
       <c r="G45" s="19">
-        <v>44104</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>92</v>
+        <v>124</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E46" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D46)</f>
-        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
+        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
       </c>
       <c r="F46" s="16">
         <v>1</v>
       </c>
       <c r="G46" s="19">
-        <v>44080</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
-        <v>132</v>
+        <v>22</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>133</v>
       </c>
       <c r="E47" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D47)</f>
-        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
+        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
       </c>
       <c r="F47" s="16">
         <v>1</v>
       </c>
-      <c r="G47" s="21">
-        <v>44067</v>
+      <c r="G47" s="19">
+        <v>44104</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2663,116 +2665,117 @@
         <v>134</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>137</v>
+      <c r="E48" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D48)</f>
+        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
       </c>
       <c r="F48" s="16">
         <v>1</v>
       </c>
-      <c r="G48" s="21">
-        <v>44066</v>
+      <c r="G48" s="19">
+        <v>44104</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>139</v>
+        <v>103</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D49)</f>
+        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
       </c>
-      <c r="G49" s="21">
-        <v>44066</v>
+      <c r="G49" s="19">
+        <v>44080</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>141</v>
+        <v>98</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E50" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D50)</f>
+        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
       </c>
       <c r="G50" s="20">
-        <v>44066</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="E51" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E51" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D51)</f>
-        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
-      </c>
       <c r="F51" s="7">
         <v>1</v>
       </c>
-      <c r="G51" s="17">
-        <v>44063</v>
+      <c r="G51" s="20">
+        <v>44066</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D52" s="12" t="s">
+      <c r="B52" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E52" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="E52" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D52)</f>
-        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
-      </c>
       <c r="F52" s="13">
         <v>1</v>
       </c>
-      <c r="G52" s="19">
-        <v>44063</v>
+      <c r="G52" s="21">
+        <v>44066</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2780,719 +2783,718 @@
         <v>146</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E53" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D53)</f>
-        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
-      </c>
       <c r="F53" s="7">
-        <v>0.97</v>
-      </c>
-      <c r="G53" s="17">
-        <v>44056</v>
+        <v>1</v>
+      </c>
+      <c r="G53" s="20">
+        <v>44066</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>111</v>
+      <c r="B54" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>149</v>
       </c>
       <c r="E54" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D54)</f>
-        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
+        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
       </c>
       <c r="F54" s="13">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="G54" s="17">
-        <v>44055</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>33</v>
+        <v>150</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E55" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D55)</f>
-        <v>https://ude.my/UC-57e2fe2c-3570-4bb3-862f-19b05a9b4413</v>
+        <v>151</v>
+      </c>
+      <c r="E55" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D55)</f>
+        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
       </c>
       <c r="F55" s="13">
         <v>1</v>
       </c>
       <c r="G55" s="17">
-        <v>44054</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>91</v>
+        <v>152</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E56" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D56)</f>
-        <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
+        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
       </c>
       <c r="F56" s="13">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G56" s="17">
-        <v>44022</v>
+        <v>44056</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>91</v>
+        <v>154</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E57" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D57)</f>
-        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
       </c>
       <c r="F57" s="13">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="G57" s="17">
-        <v>44021</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>92</v>
+        <v>31</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="E58" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D58)</f>
+      <c r="E58" s="38" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D58)</f>
+        <v>https://ude.my/UC-57e2fe2c-3570-4bb3-862f-19b05a9b4413</v>
+      </c>
+      <c r="F58" s="13">
+        <v>1</v>
+      </c>
+      <c r="G58" s="19">
+        <v>44054</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E59" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D59)</f>
+        <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
+      </c>
+      <c r="F59" s="7">
+        <v>1</v>
+      </c>
+      <c r="G59" s="17">
+        <v>44022</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E60" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D60)</f>
+        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+      </c>
+      <c r="F60" s="7">
+        <v>1</v>
+      </c>
+      <c r="G60" s="17">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E61" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D61)</f>
         <v>https://www.coursera.org/verify/L4NCNJMVFQPU</v>
       </c>
-      <c r="F58" s="13">
-        <v>1</v>
-      </c>
-      <c r="G58" s="19">
+      <c r="F61" s="7">
+        <v>1</v>
+      </c>
+      <c r="G61" s="17">
         <v>44013</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E59" s="3" t="str">
-        <f t="shared" ref="E59:E61" si="1" xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D59)</f>
+    <row r="62" spans="1:7">
+      <c r="A62" s="53" t="s">
+        <v>163</v>
+      </c>
+      <c r="B62" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="E62" s="51" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D62)</f>
         <v>https://www.hackerrank.com/certificates/867DAFFABDA4</v>
       </c>
-      <c r="F59" s="4">
-        <v>1</v>
-      </c>
-      <c r="G59" s="17">
+      <c r="F62" s="56">
+        <v>1</v>
+      </c>
+      <c r="G62" s="50">
         <v>44004</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E60" s="3" t="str">
-        <f t="shared" si="1"/>
+    <row r="63" spans="1:7">
+      <c r="A63" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E63" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D63)</f>
         <v>https://www.hackerrank.com/certificates/2766975846A6</v>
       </c>
-      <c r="F60" s="4">
-        <v>1</v>
-      </c>
-      <c r="G60" s="17">
+      <c r="F63" s="11">
+        <v>1</v>
+      </c>
+      <c r="G63" s="17">
         <v>44003</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E61" s="3" t="str">
-        <f t="shared" si="1"/>
+    <row r="64" spans="1:7">
+      <c r="A64" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E64" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D64)</f>
         <v>https://www.hackerrank.com/certificates/1140C95B9B14</v>
       </c>
-      <c r="F61" s="4">
-        <v>1</v>
-      </c>
-      <c r="G61" s="17">
+      <c r="F64" s="11">
+        <v>1</v>
+      </c>
+      <c r="G64" s="17">
         <v>44003</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B62" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D62" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="E62" s="51" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D62)</f>
-        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
-      </c>
-      <c r="F62" s="49">
-        <v>1</v>
-      </c>
-      <c r="G62" s="50">
-        <v>43999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E63" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D63)</f>
-        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
-      </c>
-      <c r="F63" s="13">
-        <v>0.94</v>
-      </c>
-      <c r="G63" s="17">
-        <v>43995</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E64" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D64)</f>
-        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
-      </c>
-      <c r="F64" s="13">
-        <v>0.94</v>
-      </c>
-      <c r="G64" s="17">
-        <v>43987</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>169</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>170</v>
       </c>
       <c r="E65" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D65)</f>
+        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
+      </c>
+      <c r="F65" s="13">
+        <v>1</v>
+      </c>
+      <c r="G65" s="19">
+        <v>43999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E66" s="10" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D66)</f>
+        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
+      </c>
+      <c r="F66" s="13">
+        <v>0.94</v>
+      </c>
+      <c r="G66" s="19">
+        <v>43995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E67" s="10" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D67)</f>
+        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+      </c>
+      <c r="F67" s="13">
+        <v>0.94</v>
+      </c>
+      <c r="G67" s="19">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E68" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D68)</f>
         <v>https://www.coursera.org/verify/3W45QQBKACKZ</v>
       </c>
-      <c r="F65" s="13">
-        <v>1</v>
-      </c>
-      <c r="G65" s="19">
+      <c r="F68" s="13">
+        <v>1</v>
+      </c>
+      <c r="G68" s="17">
         <v>43986</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="F66" s="11">
-        <v>1</v>
-      </c>
-      <c r="G66" s="19">
+    <row r="69" spans="1:7">
+      <c r="A69" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F69" s="11">
+        <v>1</v>
+      </c>
+      <c r="G69" s="17">
         <v>43984</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="F67" s="11">
-        <v>0.9</v>
-      </c>
-      <c r="G67" s="19">
-        <v>43983</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F68" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="G68" s="17">
-        <v>43983</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E69" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D69)</f>
-        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
-      </c>
-      <c r="F69" s="13">
-        <v>0.83</v>
-      </c>
-      <c r="G69" s="17">
-        <v>43983</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>91</v>
+        <v>181</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E70" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D70)</f>
-        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
+        <v>183</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="F70" s="23">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G70" s="17">
-        <v>43978</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D71" s="2" t="s">
+      <c r="F71" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="G71" s="17">
+        <v>43983</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="E71" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D71)</f>
-        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
-      </c>
-      <c r="F71" s="23">
-        <v>0.98</v>
-      </c>
-      <c r="G71" s="17">
-        <v>43968</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="2" t="s">
+      <c r="B72" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" s="2" t="s">
+      <c r="C72" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F72" s="4">
-        <v>1</v>
+      <c r="E72" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D72)</f>
+        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
+      </c>
+      <c r="F72" s="7">
+        <v>0.83</v>
       </c>
       <c r="G72" s="17">
-        <v>43965</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>195</v>
+      <c r="E73" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D73)</f>
+        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
       </c>
       <c r="F73" s="4">
         <v>1</v>
       </c>
       <c r="G73" s="17">
-        <v>43956</v>
+        <v>43978</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>197</v>
+        <v>97</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>198</v>
+        <v>98</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
+      </c>
+      <c r="E74" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D74)</f>
+        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
       </c>
       <c r="F74" s="4">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G74" s="17">
-        <v>43953</v>
+        <v>43968</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F75" s="11">
         <v>1</v>
       </c>
       <c r="G75" s="19">
-        <v>43871</v>
+        <v>43965</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>12</v>
+        <v>199</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F76" s="11">
         <v>1</v>
       </c>
       <c r="G76" s="19">
-        <v>43551</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C77" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F77" s="11">
+        <v>1</v>
+      </c>
+      <c r="G77" s="19">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B78" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C77" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="D77" s="9" t="s">
+      <c r="E78" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E77" s="10" t="s">
+      <c r="F78" s="4">
+        <v>1</v>
+      </c>
+      <c r="G78" s="17">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F77" s="11">
-        <v>1</v>
-      </c>
-      <c r="G77" s="19">
+      <c r="B79" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F79" s="4">
+        <v>1</v>
+      </c>
+      <c r="G79" s="17">
+        <v>43551</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F80" s="4">
+        <v>1</v>
+      </c>
+      <c r="G80" s="17">
         <v>43549</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E78" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D78)</f>
-        <v>https://www.hackerrank.com/certificates/eafe133d26dc</v>
-      </c>
-      <c r="F78" s="7">
-        <v>1</v>
-      </c>
-      <c r="G78" s="20">
-        <v>44469</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E79" s="6" t="str">
-        <f t="shared" ref="E79:E80" si="2" xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D79)</f>
-        <v>https://www.hackerrank.com/certificates/7a872682b210</v>
-      </c>
-      <c r="F79" s="7">
-        <v>1</v>
-      </c>
-      <c r="G79" s="20">
-        <v>44490</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D80" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="E80" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D80)</f>
-        <v>https://www.hackerrank.com/certificates/524e499db551</v>
-      </c>
-      <c r="F80" s="7">
-        <v>1</v>
-      </c>
-      <c r="G80" s="20">
-        <v>44493</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G80" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G77">
-      <sortCondition descending="1" ref="G1:G77"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G80">
+      <sortCondition descending="1" ref="G1:G80"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E77" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
-    <hyperlink ref="E76" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
-    <hyperlink ref="E75" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
-    <hyperlink ref="E73" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
-    <hyperlink ref="E74" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
-    <hyperlink ref="E71" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
-    <hyperlink ref="E72" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
-    <hyperlink ref="E66" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
-    <hyperlink ref="E67" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
-    <hyperlink ref="E68" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
-    <hyperlink ref="E60" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
-    <hyperlink ref="E61" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
-    <hyperlink ref="E59" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
-    <hyperlink ref="E33" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
-    <hyperlink ref="E31" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
-    <hyperlink ref="E28" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
-    <hyperlink ref="E27" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
-    <hyperlink ref="E26" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
-    <hyperlink ref="E25" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
-    <hyperlink ref="E7" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
-    <hyperlink ref="E4" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
-    <hyperlink ref="E5" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
-    <hyperlink ref="E2" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
-    <hyperlink ref="E8" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
-    <hyperlink ref="E12" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
-    <hyperlink ref="E17" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
-    <hyperlink ref="E20" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
-    <hyperlink ref="E21" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
-    <hyperlink ref="E22" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
-    <hyperlink ref="E18" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
-    <hyperlink ref="E19" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
-    <hyperlink ref="E23" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
-    <hyperlink ref="E29" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
-    <hyperlink ref="E48" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
-    <hyperlink ref="E49" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
-    <hyperlink ref="E50" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
-    <hyperlink ref="E3" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
-    <hyperlink ref="E70" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
+    <hyperlink ref="E80" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
+    <hyperlink ref="E79" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
+    <hyperlink ref="E78" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
+    <hyperlink ref="E76" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
+    <hyperlink ref="E77" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
+    <hyperlink ref="E74" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
+    <hyperlink ref="E75" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
+    <hyperlink ref="E69" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
+    <hyperlink ref="E70" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
+    <hyperlink ref="E71" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
+    <hyperlink ref="E63" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
+    <hyperlink ref="E64" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
+    <hyperlink ref="E62" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
+    <hyperlink ref="E36" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
+    <hyperlink ref="E34" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
+    <hyperlink ref="E31" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
+    <hyperlink ref="E30" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
+    <hyperlink ref="E29" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
+    <hyperlink ref="E28" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
+    <hyperlink ref="E10" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
+    <hyperlink ref="E7" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
+    <hyperlink ref="E8" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
+    <hyperlink ref="E9" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
+    <hyperlink ref="E11" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
+    <hyperlink ref="E15" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
+    <hyperlink ref="E20" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
+    <hyperlink ref="E23" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
+    <hyperlink ref="E24" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
+    <hyperlink ref="E25" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
+    <hyperlink ref="E21" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
+    <hyperlink ref="E22" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
+    <hyperlink ref="E26" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
+    <hyperlink ref="E32" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
+    <hyperlink ref="E51" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
+    <hyperlink ref="E52" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
+    <hyperlink ref="E53" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
+    <hyperlink ref="E6" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
+    <hyperlink ref="E73" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
     <hyperlink ref="E29:E42" r:id="rId39" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{CE0B26B0-E940-4BD5-8F74-8D28A4F3B13A}"/>
-    <hyperlink ref="E30" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
-    <hyperlink ref="E47" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
-    <hyperlink ref="E9" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
+    <hyperlink ref="E33" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
+    <hyperlink ref="E50" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
+    <hyperlink ref="E12" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
     <hyperlink ref="E9:E10" r:id="rId43" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{C55AB7BE-0BE1-4CE1-8CFE-C0E7B2B0BA28}"/>
     <hyperlink ref="E12:E15" r:id="rId44" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{549C4CBA-43AF-4870-BE36-8D1CBC3CFD71}"/>
-    <hyperlink ref="E24" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
-    <hyperlink ref="E55" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
-    <hyperlink ref="E6" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
-    <hyperlink ref="E78" r:id="rId48" display="https://www.hackerrank.com/certificates/eafe133d26dc" xr:uid="{3748E750-A80A-4402-BC5F-803B16F27441}"/>
+    <hyperlink ref="E27" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
+    <hyperlink ref="E58" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
+    <hyperlink ref="E5" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
+    <hyperlink ref="E4" r:id="rId48" display="https://www.hackerrank.com/certificates/eafe133d26dc" xr:uid="{3748E750-A80A-4402-BC5F-803B16F27441}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3825,7 +3827,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B5" s="7">
         <v>0.8</v>

</xml_diff>

<commit_message>
Fixed typos and bugs
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24715"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B9DCE1D-BB74-4E44-B2A1-C9DF91B6D3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DE885E0-F16E-4C03-9D20-D04669549040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certifications" sheetId="1" r:id="rId1"/>
@@ -3563,8 +3563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7494C2C-9786-4889-8081-3FC41A1A3B3E}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3625,7 +3625,7 @@
         <v>227</v>
       </c>
       <c r="F2" s="30">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="G2" s="30" t="s">
         <v>227</v>
@@ -4048,7 +4048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DB9CC9-BE76-4E73-A91C-99466DD45DAE}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
@@ -4286,12 +4286,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C797B8AD90D44498DEE196080AFE3F2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d8a7b83c41275397db5e03f2b73eca8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fefa867-d15f-4a0d-9945-ea6297accf67" xmlns:ns3="fadb6cc6-1edc-4022-b9cc-b0c463f8d195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fb96d3b9dc267ba3c8d7f8af4b53bea" ns2:_="" ns3:_="">
     <xsd:import namespace="0fefa867-d15f-4a0d-9945-ea6297accf67"/>
@@ -4508,14 +4502,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
 </file>
</xml_diff>

<commit_message>
Added AI 900 Certification
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24722"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DE885E0-F16E-4C03-9D20-D04669549040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF858760-F757-4B8E-A7CC-3B57758DE4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certifications" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Certifications!$A$1:$G$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Experience!$A$1:$I$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Skills!$A$1:$B$22</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="316">
   <si>
     <t>Title</t>
   </si>
@@ -56,6 +57,18 @@
     <t>IssuedOn</t>
   </si>
   <si>
+    <t>Microsoft Certified: Azure AI Fundamentals</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>I045-9367</t>
+  </si>
+  <si>
+    <t>https://www.credly.com/badges/bee3fafd-9644-4783-b3b0-3b96c0373e4c</t>
+  </si>
+  <si>
     <t>JavaScript (Intermediate)</t>
   </si>
   <si>
@@ -80,9 +93,6 @@
     <t>Microsoft Certified: Azure Data Fundamentals</t>
   </si>
   <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
     <t>H918-4797</t>
   </si>
   <si>
@@ -791,55 +801,61 @@
     <t>PYTHON</t>
   </si>
   <si>
+    <t>AZURE SYNAPSE</t>
+  </si>
+  <si>
+    <t>DJANGO</t>
+  </si>
+  <si>
+    <t>JAVA SCRIPT</t>
+  </si>
+  <si>
+    <t>SQL DATABASE</t>
+  </si>
+  <si>
+    <t>TKINTER</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>JQUERY</t>
+  </si>
+  <si>
+    <t>NODE JS</t>
+  </si>
+  <si>
+    <t>REACT JS</t>
+  </si>
+  <si>
+    <t>BOOTSTRAP</t>
+  </si>
+  <si>
     <t>CSS</t>
   </si>
   <si>
-    <t>BOOTSTRAP</t>
-  </si>
-  <si>
-    <t>JQUERY</t>
-  </si>
-  <si>
-    <t>DJANGO</t>
-  </si>
-  <si>
-    <t>TKINTER</t>
-  </si>
-  <si>
-    <t>SQL DATABASE</t>
-  </si>
-  <si>
-    <t>REACT JS</t>
-  </si>
-  <si>
-    <t>NODE JS</t>
-  </si>
-  <si>
-    <t>JAVA SCRIPT</t>
-  </si>
-  <si>
-    <t>AZURE SYNAPSE</t>
+    <t>GIT</t>
+  </si>
+  <si>
+    <t>PYQT5</t>
+  </si>
+  <si>
+    <t>SHAREPOINT</t>
+  </si>
+  <si>
+    <t>WEB SCRAPING</t>
   </si>
   <si>
     <t>WORDPRESS</t>
   </si>
   <si>
-    <t>SHAREPOINT</t>
-  </si>
-  <si>
-    <t>GIT</t>
-  </si>
-  <si>
     <t>POWER APPS</t>
   </si>
   <si>
+    <t>POWER AUTOMATE</t>
+  </si>
+  <si>
     <t>POWER BI</t>
-  </si>
-  <si>
-    <t>C#</t>
-  </si>
-  <si>
-    <t>PYQT5</t>
   </si>
   <si>
     <t>ProjectURL</t>
@@ -1145,7 +1161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1173,8 +1189,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1205,7 +1219,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1220,10 +1233,10 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1539,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1580,132 +1593,132 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="39" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D2)</f>
-        <v>https://www.hackerrank.com/certificates/524e499db551</v>
-      </c>
-      <c r="F2" s="40">
-        <v>1</v>
-      </c>
-      <c r="G2" s="30">
-        <v>44493</v>
+      <c r="E2" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="37">
+        <v>0.98</v>
+      </c>
+      <c r="G2" s="28">
+        <v>44527</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>13</v>
       </c>
       <c r="E3" s="6" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D3)</f>
+        <v>https://www.hackerrank.com/certificates/524e499db551</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="20">
+        <v>44493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="35" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D4)</f>
         <v>https://www.hackerrank.com/certificates/7a872682b210</v>
       </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="20">
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21">
         <v>44490</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="38" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D4)</f>
-        <v>https://www.hackerrank.com/certificates/eafe133d26dc</v>
-      </c>
-      <c r="F4" s="13">
-        <v>1</v>
-      </c>
-      <c r="G4" s="21">
-        <v>44469</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="E5" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D5)</f>
+        <v>https://www.hackerrank.com/certificates/eafe133d26dc</v>
+      </c>
       <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="20">
+        <v>44469</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="37">
         <v>0.94</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G6" s="28">
         <v>44439</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="40">
-        <v>1</v>
-      </c>
-      <c r="G6" s="30">
-        <v>44419</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -1717,29 +1730,29 @@
         <v>1</v>
       </c>
       <c r="G7" s="20">
-        <v>44418</v>
+        <v>44419</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20">
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="21">
         <v>44418</v>
       </c>
     </row>
@@ -1748,10 +1761,10 @@
         <v>28</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>29</v>
@@ -1760,33 +1773,33 @@
         <v>30</v>
       </c>
       <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20">
+        <v>44418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="43">
         <v>0.88</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G10" s="42">
         <v>44412</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="13">
-        <v>1</v>
-      </c>
-      <c r="G10" s="21">
-        <v>44388</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1794,71 +1807,70 @@
         <v>34</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="6" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D11)</f>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="20">
+        <v>44388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="36" t="str">
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D12)</f>
         <v>https://verify.greatlearning.in/UAEGKOSB</v>
       </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="20">
+      <c r="F12" s="37">
+        <v>1</v>
+      </c>
+      <c r="G12" s="28">
         <v>44348</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="39" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D12)</f>
-        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
-      </c>
-      <c r="F12" s="40">
-        <v>1</v>
-      </c>
-      <c r="G12" s="30">
-        <v>44346</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D13)</f>
-        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
+        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
       </c>
       <c r="F13" s="7">
         <v>1</v>
       </c>
       <c r="G13" s="20">
-        <v>44339</v>
+        <v>44346</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1869,20 +1881,20 @@
         <v>45</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D14)</f>
-        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
+        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
       </c>
       <c r="G14" s="20">
-        <v>44332</v>
+        <v>44339</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1893,37 +1905,37 @@
         <v>48</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>50</v>
+      <c r="E15" s="6" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D15)</f>
+        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
       </c>
       <c r="F15" s="13">
         <v>1</v>
       </c>
       <c r="G15" s="21">
-        <v>44312</v>
+        <v>44332</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="C16" s="12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="38" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D16)</f>
-        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
+      <c r="E16" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="F16" s="13">
         <v>1</v>
@@ -1934,26 +1946,26 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E17" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D17)</f>
-        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
+        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
       </c>
       <c r="F17" s="7">
         <v>1</v>
       </c>
       <c r="G17" s="20">
-        <v>44309</v>
+        <v>44312</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1964,20 +1976,20 @@
         <v>57</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D18)</f>
-        <v>https://ude.my/UC-1f46a0d1-37f4-4a8c-95f6-839311438ab7</v>
+        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="G18" s="20">
-        <v>44306</v>
+        <v>44309</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1988,62 +2000,62 @@
         <v>60</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D19)</f>
+        <v>https://ude.my/UC-1f46a0d1-37f4-4a8c-95f6-839311438ab7</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="20">
+        <v>44306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="36" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D20)</f>
         <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
       </c>
-      <c r="F19" s="7">
-        <v>1</v>
-      </c>
-      <c r="G19" s="20">
+      <c r="F20" s="37">
+        <v>1</v>
+      </c>
+      <c r="G20" s="28">
         <v>44300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="39" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D20)</f>
-        <v>https://www.hackerrank.com/certificates/cf58231a440f</v>
-      </c>
-      <c r="F20" s="40">
-        <v>1</v>
-      </c>
-      <c r="G20" s="30">
-        <v>44288</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" s="6" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D21)</f>
-        <v>https://www.hackerrank.com/certificates/4490b4a0e606</v>
+        <v>https://www.hackerrank.com/certificates/cf58231a440f</v>
       </c>
       <c r="F21" s="13">
         <v>1</v>
@@ -2054,20 +2066,20 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="38" t="str">
+        <v>68</v>
+      </c>
+      <c r="E22" s="35" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D22)</f>
-        <v>https://www.hackerrank.com/certificates/fdeeaad81310</v>
+        <v>https://www.hackerrank.com/certificates/4490b4a0e606</v>
       </c>
       <c r="F22" s="13">
         <v>1</v>
@@ -2078,44 +2090,44 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E23" s="6" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D23)</f>
-        <v>https://verify.greatlearning.in/SSMRYOWJ</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D23)</f>
+        <v>https://www.hackerrank.com/certificates/fdeeaad81310</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
       </c>
       <c r="G23" s="20">
-        <v>44287</v>
+        <v>44288</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E24" s="6" t="str">
         <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D24)</f>
-        <v>https://verify.greatlearning.in/ZYQTXTJA</v>
+        <v>https://verify.greatlearning.in/SSMRYOWJ</v>
       </c>
       <c r="F24" s="7">
         <v>1</v>
@@ -2126,20 +2138,20 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E25" s="6" t="str">
         <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D25)</f>
-        <v>https://verify.greatlearning.in/GQGRZFQQ</v>
+        <v>https://verify.greatlearning.in/ZYQTXTJA</v>
       </c>
       <c r="F25" s="7">
         <v>1</v>
@@ -2149,75 +2161,75 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="28" t="s">
+      <c r="A26" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="39" t="str">
+      <c r="B26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="36" t="str">
         <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D26)</f>
+        <v>https://verify.greatlearning.in/GQGRZFQQ</v>
+      </c>
+      <c r="F26" s="37">
+        <v>1</v>
+      </c>
+      <c r="G26" s="28">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="36" t="str">
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D27)</f>
         <v>https://verify.greatlearning.in/HSNELKCZ</v>
       </c>
-      <c r="F26" s="40">
-        <v>1</v>
-      </c>
-      <c r="G26" s="30">
+      <c r="F27" s="43">
+        <v>1</v>
+      </c>
+      <c r="G27" s="42">
         <v>44287</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="39" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D27)</f>
-        <v>https://www.hackerrank.com/certificates/1cadc360a79d</v>
-      </c>
-      <c r="F27" s="46">
-        <v>1</v>
-      </c>
-      <c r="G27" s="45">
-        <v>44268</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>80</v>
       </c>
       <c r="E28" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D28)</f>
-        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D28)</f>
+        <v>https://www.hackerrank.com/certificates/1cadc360a79d</v>
       </c>
       <c r="F28" s="13">
         <v>1</v>
       </c>
       <c r="G28" s="21">
-        <v>44249</v>
+        <v>44268</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2228,184 +2240,184 @@
         <v>82</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>84</v>
+      <c r="E29" s="6" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D29)</f>
+        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
       </c>
       <c r="F29" s="13">
-        <v>0.97</v>
-      </c>
-      <c r="G29" s="17">
-        <v>44246</v>
+        <v>1</v>
+      </c>
+      <c r="G29" s="20">
+        <v>44249</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="C30" s="12" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="38" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D30)</f>
-        <v>https://www.hackerrank.com/certificates/6730CF1D0F21</v>
+      <c r="E30" s="35" t="s">
+        <v>87</v>
       </c>
       <c r="F30" s="13">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G30" s="19">
-        <v>44209</v>
+        <v>44246</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="6" t="s">
         <v>89</v>
       </c>
+      <c r="E31" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D31)</f>
+        <v>https://www.hackerrank.com/certificates/6730CF1D0F21</v>
+      </c>
       <c r="F31" s="7">
         <v>1</v>
       </c>
       <c r="G31" s="17">
+        <v>44209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="37">
+        <v>1</v>
+      </c>
+      <c r="G32" s="47">
         <v>44180</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="52">
-        <v>271676</v>
-      </c>
-      <c r="E32" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" s="40">
-        <v>1</v>
-      </c>
-      <c r="G32" s="53">
-        <v>44176</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D33" s="8">
         <v>271676</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
-      <c r="G33" s="20">
+      <c r="G33" s="17">
         <v>44176</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="8">
+        <v>271676</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D34)</f>
-        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
-      </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
-      <c r="G34" s="17">
-        <v>44165</v>
+      <c r="G34" s="20">
+        <v>44176</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="C35" s="12" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D35)</f>
-        <v>https://www.hackerrank.com/certificates/3AF4DDB28FAB</v>
+        <v>100</v>
+      </c>
+      <c r="E35" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D35)</f>
+        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
       </c>
       <c r="F35" s="13">
         <v>1</v>
       </c>
       <c r="G35" s="19">
-        <v>44146</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D36)</f>
-        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
+      <c r="E36" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D36)</f>
+        <v>https://www.hackerrank.com/certificates/3AF4DDB28FAB</v>
       </c>
       <c r="F36" s="7">
         <v>1</v>
       </c>
       <c r="G36" s="19">
-        <v>44135</v>
+        <v>44146</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2416,13 +2428,14 @@
         <v>104</v>
       </c>
       <c r="C37" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>107</v>
+      <c r="E37" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D37)</f>
+        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
       </c>
       <c r="F37" s="7">
         <v>1</v>
@@ -2433,44 +2446,43 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>96</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D38)</f>
-        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
+      <c r="E38" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
       </c>
       <c r="G38" s="19">
-        <v>44126</v>
+        <v>44135</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E39" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D39)</f>
-        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
+        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
@@ -2481,20 +2493,20 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E40" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D40)</f>
-        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D40)</f>
+        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
@@ -2505,26 +2517,26 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>116</v>
       </c>
       <c r="E41" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D41)</f>
-        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D41)</f>
+        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
       </c>
       <c r="F41" s="7">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G41" s="19">
-        <v>44124</v>
+        <v>44126</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2532,20 +2544,20 @@
         <v>117</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D42)</f>
-        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D42)</f>
+        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
       </c>
       <c r="F42" s="16">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G42" s="19">
         <v>44124</v>
@@ -2553,47 +2565,47 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E43" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D43)</f>
-        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D43)</f>
+        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
       </c>
       <c r="F43" s="16">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G43" s="19">
-        <v>44122</v>
+        <v>44124</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>123</v>
       </c>
       <c r="E44" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D44)</f>
-        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D44)</f>
+        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
       </c>
       <c r="F44" s="16">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G44" s="19">
         <v>44122</v>
@@ -2607,20 +2619,20 @@
         <v>125</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>126</v>
       </c>
       <c r="E45" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D45)</f>
-        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D45)</f>
+        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
       </c>
       <c r="F45" s="16">
         <v>1</v>
       </c>
       <c r="G45" s="19">
-        <v>44112</v>
+        <v>44122</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2628,41 +2640,41 @@
         <v>127</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E46" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D46)</f>
-        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
+        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
       </c>
       <c r="F46" s="16">
         <v>1</v>
       </c>
       <c r="G46" s="19">
-        <v>44105</v>
+        <v>44112</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E47" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D47)</f>
-        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
+        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
       </c>
       <c r="F47" s="16">
         <v>1</v>
@@ -2673,68 +2685,68 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E48" s="6" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D48)</f>
-        <v>https://verify.greatlearning.in/UYEYVCWB</v>
+        <v>133</v>
+      </c>
+      <c r="E48" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D48)</f>
+        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
       </c>
       <c r="F48" s="16">
         <v>1</v>
       </c>
-      <c r="G48" s="21">
+      <c r="G48" s="19">
         <v>44105</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>122</v>
+        <v>38</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E49" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D49)</f>
-        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
+        <v>134</v>
+      </c>
+      <c r="E49" s="6" t="str">
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D49)</f>
+        <v>https://verify.greatlearning.in/UYEYVCWB</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
       </c>
-      <c r="G49" s="19">
-        <v>44104</v>
+      <c r="G49" s="21">
+        <v>44105</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
-        <v>133</v>
+        <v>25</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E50" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D50)</f>
-        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
+        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
@@ -2745,90 +2757,91 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>96</v>
+        <v>125</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E51" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D51)</f>
-        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
+        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
       </c>
       <c r="F51" s="7">
         <v>1</v>
       </c>
       <c r="G51" s="17">
-        <v>44080</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>96</v>
+        <v>104</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E52" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D52)</f>
-        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
+        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
       </c>
       <c r="F52" s="13">
         <v>1</v>
       </c>
-      <c r="G52" s="21">
-        <v>44067</v>
+      <c r="G52" s="19">
+        <v>44080</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D53" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>142</v>
+      <c r="E53" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D53)</f>
+        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
       </c>
       <c r="F53" s="7">
         <v>1</v>
       </c>
       <c r="G53" s="20">
-        <v>44066</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="C54" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F54" s="13">
         <v>1</v>
@@ -2839,19 +2852,19 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F55" s="13">
         <v>1</v>
@@ -2862,44 +2875,43 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D56" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E56" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D56)</f>
-        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
+      <c r="B56" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="F56" s="13">
         <v>1</v>
       </c>
-      <c r="G56" s="17">
-        <v>44063</v>
+      <c r="G56" s="20">
+        <v>44066</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E57" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D57)</f>
-        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D57)</f>
+        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
       </c>
       <c r="F57" s="13">
         <v>1</v>
@@ -2910,212 +2922,212 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>115</v>
+        <v>152</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E58" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D58)</f>
-        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D58)</f>
+        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
       </c>
       <c r="F58" s="13">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G58" s="19">
-        <v>44056</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E59" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D59)</f>
-        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
+        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
       </c>
       <c r="F59" s="7">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="G59" s="17">
-        <v>44055</v>
+        <v>44056</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="5" t="s">
-        <v>31</v>
+        <v>156</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>39</v>
+        <v>118</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="E60" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D60)</f>
-        <v>https://ude.my/UC-57e2fe2c-3570-4bb3-862f-19b05a9b4413</v>
+        <v>157</v>
+      </c>
+      <c r="E60" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D60)</f>
+        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
       </c>
       <c r="F60" s="7">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="G60" s="17">
-        <v>44054</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>96</v>
+        <v>34</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E61" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D61)</f>
+        <v>158</v>
+      </c>
+      <c r="E61" s="6" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D61)</f>
+        <v>https://ude.my/UC-57e2fe2c-3570-4bb3-862f-19b05a9b4413</v>
+      </c>
+      <c r="F61" s="7">
+        <v>1</v>
+      </c>
+      <c r="G61" s="17">
+        <v>44054</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="E62" s="45" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D62)</f>
         <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
       </c>
-      <c r="F61" s="7">
-        <v>1</v>
-      </c>
-      <c r="G61" s="17">
+      <c r="F62" s="43">
+        <v>1</v>
+      </c>
+      <c r="G62" s="44">
         <v>44022</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="B62" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D62" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="E62" s="48" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D62)</f>
-        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
-      </c>
-      <c r="F62" s="46">
-        <v>1</v>
-      </c>
-      <c r="G62" s="47">
-        <v>44021</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E63" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D63)</f>
+        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+      </c>
+      <c r="F63" s="13">
+        <v>1</v>
+      </c>
+      <c r="G63" s="17">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E64" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D64)</f>
         <v>https://www.coursera.org/verify/L4NCNJMVFQPU</v>
       </c>
-      <c r="F63" s="13">
-        <v>1</v>
-      </c>
-      <c r="G63" s="17">
+      <c r="F64" s="13">
+        <v>1</v>
+      </c>
+      <c r="G64" s="17">
         <v>44013</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E64" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D64)</f>
-        <v>https://www.hackerrank.com/certificates/867DAFFABDA4</v>
-      </c>
-      <c r="F64" s="11">
-        <v>1</v>
-      </c>
-      <c r="G64" s="17">
-        <v>44004</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E65" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D65)</f>
-        <v>https://www.hackerrank.com/certificates/2766975846A6</v>
+        <v>https://www.hackerrank.com/certificates/867DAFFABDA4</v>
       </c>
       <c r="F65" s="11">
         <v>1</v>
       </c>
       <c r="G65" s="19">
-        <v>44003</v>
+        <v>44004</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E66" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D66)</f>
-        <v>https://www.hackerrank.com/certificates/1140C95B9B14</v>
+        <v>https://www.hackerrank.com/certificates/2766975846A6</v>
       </c>
       <c r="F66" s="11">
         <v>1</v>
@@ -3125,75 +3137,75 @@
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="12" t="s">
-        <v>22</v>
+      <c r="A67" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>168</v>
+        <v>12</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="E67" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D67)</f>
-        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
-      </c>
-      <c r="F67" s="13">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D67)</f>
+        <v>https://www.hackerrank.com/certificates/1140C95B9B14</v>
+      </c>
+      <c r="F67" s="11">
         <v>1</v>
       </c>
       <c r="G67" s="19">
-        <v>43999</v>
+        <v>44003</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>96</v>
+        <v>25</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E68" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D68)</f>
-        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
+        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
       </c>
       <c r="F68" s="13">
-        <v>0.94</v>
+        <v>1</v>
       </c>
       <c r="G68" s="17">
-        <v>43995</v>
+        <v>43999</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>172</v>
+        <v>104</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E69" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D69)</f>
-        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
       </c>
       <c r="F69" s="13">
         <v>0.94</v>
       </c>
       <c r="G69" s="17">
-        <v>43987</v>
+        <v>43995</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3201,46 +3213,47 @@
         <v>174</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E70" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D70)</f>
+        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+      </c>
+      <c r="F70" s="16">
+        <v>0.94</v>
+      </c>
+      <c r="G70" s="17">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E71" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D71)</f>
         <v>https://www.coursera.org/verify/3W45QQBKACKZ</v>
       </c>
-      <c r="F70" s="16">
-        <v>1</v>
-      </c>
-      <c r="G70" s="17">
+      <c r="F71" s="16">
+        <v>1</v>
+      </c>
+      <c r="G71" s="17">
         <v>43986</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F71" s="23">
-        <v>1</v>
-      </c>
-      <c r="G71" s="17">
-        <v>43984</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3248,33 +3261,33 @@
         <v>179</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="E72" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="F72" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G72" s="17">
-        <v>43983</v>
+        <v>43984</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>185</v>
@@ -3283,105 +3296,105 @@
         <v>186</v>
       </c>
       <c r="F73" s="4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G73" s="17">
         <v>43983</v>
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="24" t="s">
+      <c r="A74" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D74" s="5" t="s">
+      <c r="E74" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E74" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D74)</f>
-        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
-      </c>
-      <c r="F74" s="7">
-        <v>0.83</v>
+      <c r="F74" s="4">
+        <v>0.8</v>
       </c>
       <c r="G74" s="17">
         <v>43983</v>
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="B75" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D75" s="9" t="s">
+      <c r="B75" s="12" t="s">
         <v>191</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>192</v>
       </c>
       <c r="E75" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D75)</f>
-        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
-      </c>
-      <c r="F75" s="11">
-        <v>1</v>
+        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
+      </c>
+      <c r="F75" s="13">
+        <v>0.83</v>
       </c>
       <c r="G75" s="19">
-        <v>43978</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B76" s="25" t="s">
-        <v>95</v>
+        <v>193</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E76" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D76)</f>
-        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
+        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
       </c>
       <c r="F76" s="11">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G76" s="19">
-        <v>43968</v>
+        <v>43978</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C77" s="43" t="s">
-        <v>19</v>
+        <v>98</v>
+      </c>
+      <c r="C77" s="40" t="s">
+        <v>99</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E77" s="10" t="s">
         <v>196</v>
       </c>
+      <c r="E77" s="10" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D77)</f>
+        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
+      </c>
       <c r="F77" s="11">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G77" s="19">
-        <v>43965</v>
+        <v>43968</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3389,56 +3402,56 @@
         <v>197</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D78" s="2" t="s">
+      <c r="E78" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="F78" s="4">
         <v>1</v>
       </c>
       <c r="G78" s="17">
-        <v>43956</v>
+        <v>43965</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="E79" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="F79" s="4">
         <v>1</v>
       </c>
       <c r="G79" s="17">
-        <v>43953</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>206</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>207</v>
@@ -3450,7 +3463,7 @@
         <v>1</v>
       </c>
       <c r="G80" s="19">
-        <v>43871</v>
+        <v>43953</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3458,10 +3471,10 @@
         <v>209</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>210</v>
@@ -3473,87 +3486,111 @@
         <v>1</v>
       </c>
       <c r="G81" s="17">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F82" s="11">
+        <v>1</v>
+      </c>
+      <c r="G82" s="19">
         <v>43551</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E82" s="3" t="s">
+    <row r="83" spans="1:7">
+      <c r="A83" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F82" s="4">
-        <v>1</v>
-      </c>
-      <c r="G82" s="17">
+      <c r="B83" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F83" s="4">
+        <v>1</v>
+      </c>
+      <c r="G83" s="17">
         <v>43549</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G82" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G82">
-      <sortCondition descending="1" ref="G1:G82"/>
+  <autoFilter ref="A1:G83" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G83">
+      <sortCondition descending="1" ref="G1:G83"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E82" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
-    <hyperlink ref="E81" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
-    <hyperlink ref="E80" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
-    <hyperlink ref="E78" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
-    <hyperlink ref="E79" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
-    <hyperlink ref="E76" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
-    <hyperlink ref="E77" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
-    <hyperlink ref="E71" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
-    <hyperlink ref="E72" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
-    <hyperlink ref="E73" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
-    <hyperlink ref="E65" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
-    <hyperlink ref="E66" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
-    <hyperlink ref="E64" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
-    <hyperlink ref="E37" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
-    <hyperlink ref="E35" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
-    <hyperlink ref="E32" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
-    <hyperlink ref="E31" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
-    <hyperlink ref="E30" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
-    <hyperlink ref="E29" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
-    <hyperlink ref="E10" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
-    <hyperlink ref="E7" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
-    <hyperlink ref="E8" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
-    <hyperlink ref="E9" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
-    <hyperlink ref="E11" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
-    <hyperlink ref="E15" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
-    <hyperlink ref="E20" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
-    <hyperlink ref="E23" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
-    <hyperlink ref="E24" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
-    <hyperlink ref="E25" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
-    <hyperlink ref="E21" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
-    <hyperlink ref="E22" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
-    <hyperlink ref="E27" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
-    <hyperlink ref="E33" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
-    <hyperlink ref="E53" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
-    <hyperlink ref="E54" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
-    <hyperlink ref="E55" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
-    <hyperlink ref="E6" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
-    <hyperlink ref="E75" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
+    <hyperlink ref="E83" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
+    <hyperlink ref="E82" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
+    <hyperlink ref="E81" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
+    <hyperlink ref="E79" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
+    <hyperlink ref="E80" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
+    <hyperlink ref="E77" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
+    <hyperlink ref="E78" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
+    <hyperlink ref="E72" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
+    <hyperlink ref="E73" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
+    <hyperlink ref="E74" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
+    <hyperlink ref="E66" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
+    <hyperlink ref="E67" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
+    <hyperlink ref="E65" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
+    <hyperlink ref="E38" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
+    <hyperlink ref="E36" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
+    <hyperlink ref="E33" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
+    <hyperlink ref="E32" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
+    <hyperlink ref="E31" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
+    <hyperlink ref="E30" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
+    <hyperlink ref="E11" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
+    <hyperlink ref="E8" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
+    <hyperlink ref="E9" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
+    <hyperlink ref="E10" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
+    <hyperlink ref="E12" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
+    <hyperlink ref="E16" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
+    <hyperlink ref="E21" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
+    <hyperlink ref="E24" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
+    <hyperlink ref="E25" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
+    <hyperlink ref="E26" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
+    <hyperlink ref="E22" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
+    <hyperlink ref="E23" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
+    <hyperlink ref="E28" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
+    <hyperlink ref="E34" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
+    <hyperlink ref="E54" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
+    <hyperlink ref="E55" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
+    <hyperlink ref="E56" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
+    <hyperlink ref="E7" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
+    <hyperlink ref="E76" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
     <hyperlink ref="E29:E42" r:id="rId39" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{CE0B26B0-E940-4BD5-8F74-8D28A4F3B13A}"/>
-    <hyperlink ref="E34" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
-    <hyperlink ref="E52" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
-    <hyperlink ref="E12" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
+    <hyperlink ref="E35" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
+    <hyperlink ref="E53" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
+    <hyperlink ref="E13" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
     <hyperlink ref="E9:E10" r:id="rId43" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{C55AB7BE-0BE1-4CE1-8CFE-C0E7B2B0BA28}"/>
     <hyperlink ref="E12:E15" r:id="rId44" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{549C4CBA-43AF-4870-BE36-8D1CBC3CFD71}"/>
-    <hyperlink ref="E28" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
-    <hyperlink ref="E60" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
-    <hyperlink ref="E5" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
-    <hyperlink ref="E4" r:id="rId48" display="https://www.hackerrank.com/certificates/eafe133d26dc" xr:uid="{3748E750-A80A-4402-BC5F-803B16F27441}"/>
+    <hyperlink ref="E29" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
+    <hyperlink ref="E61" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
+    <hyperlink ref="E6" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
+    <hyperlink ref="E5" r:id="rId48" display="https://www.hackerrank.com/certificates/eafe133d26dc" xr:uid="{3748E750-A80A-4402-BC5F-803B16F27441}"/>
+    <hyperlink ref="E2" r:id="rId49" xr:uid="{59D89928-3553-4495-8CD7-92EBC3B422E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3563,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7494C2C-9786-4889-8081-3FC41A1A3B3E}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3581,27 +3618,27 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>221</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>220</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="G1" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="E1" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -3610,73 +3647,73 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="F2" s="30">
+      <c r="C2" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" s="28">
         <v>44470</v>
       </c>
-      <c r="G2" s="30" t="s">
-        <v>227</v>
+      <c r="G2" s="28" t="s">
+        <v>230</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="28">
+        <v>44378</v>
+      </c>
+      <c r="G3" s="28">
+        <v>44469</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="F3" s="30">
-        <v>44378</v>
-      </c>
-      <c r="G3" s="30">
-        <v>44469</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>231</v>
+        <v>235</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>234</v>
       </c>
       <c r="F4" s="20">
         <v>44263</v>
@@ -3685,54 +3722,54 @@
         <v>44377</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" s="36" customFormat="1" ht="75">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:9" s="34" customFormat="1" ht="75">
+      <c r="A5" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="E5" s="33" t="s">
+      <c r="F5" s="32">
+        <v>44137</v>
+      </c>
+      <c r="G5" s="32">
+        <v>44200</v>
+      </c>
+      <c r="H5" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="F5" s="34">
-        <v>44137</v>
-      </c>
-      <c r="G5" s="34">
-        <v>44200</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>237</v>
+      <c r="I5" s="33" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>231</v>
+        <v>242</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>234</v>
       </c>
       <c r="F6" s="20">
         <v>44136</v>
@@ -3741,27 +3778,27 @@
         <v>44166</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>231</v>
+      <c r="C7" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>234</v>
       </c>
       <c r="F7" s="20">
         <v>44105</v>
@@ -3770,27 +3807,27 @@
         <v>44136</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>231</v>
+        <v>250</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>234</v>
       </c>
       <c r="F8" s="20">
         <v>43432</v>
@@ -3799,10 +3836,10 @@
         <v>43442</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3867,29 +3904,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718451B2-E12D-4ABD-B26C-5975AED3964E}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>250</v>
+      <c r="A1" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B2" s="7">
         <v>0.9</v>
@@ -3897,23 +3932,23 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B3" s="7">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B4" s="7">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>206</v>
+      <c r="A5" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="B5" s="7">
         <v>0.8</v>
@@ -3921,15 +3956,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B6" s="7">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B7" s="7">
         <v>0.8</v>
@@ -3937,7 +3972,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B8" s="7">
         <v>0.8</v>
@@ -3945,101 +3980,122 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B9" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B10" s="7">
         <v>0.7</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="B11" s="13">
+      <c r="A11" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B11" s="7">
         <v>0.7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="B12" s="13">
-        <v>0.8</v>
+      <c r="A12" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="B13" s="16">
-        <v>0.8</v>
+      <c r="A13" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="B14" s="13">
+      <c r="A14" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" s="7">
         <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="B15" s="13">
+      <c r="A15" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" s="7">
         <v>0.6</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="B16" s="13">
+      <c r="A16" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B16" s="7">
         <v>0.6</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B17" s="7">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="B18" s="13">
-        <v>0.5</v>
+      <c r="A18" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0.6</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="B19" s="13">
-        <v>0.7</v>
+      <c r="A19" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B20" s="7">
-        <v>0.6</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B22" xr:uid="{718451B2-E12D-4ABD-B26C-5975AED3964E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B22">
+      <sortCondition descending="1" ref="B1:B22"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4048,8 +4104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DB9CC9-BE76-4E73-A91C-99466DD45DAE}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="A1:D14"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4061,199 +4117,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
-        <v>249</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>269</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>270</v>
+      <c r="B1" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4286,6 +4342,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C797B8AD90D44498DEE196080AFE3F2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d8a7b83c41275397db5e03f2b73eca8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fefa867-d15f-4a0d-9945-ea6297accf67" xmlns:ns3="fadb6cc6-1edc-4022-b9cc-b0c463f8d195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fb96d3b9dc267ba3c8d7f8af4b53bea" ns2:_="" ns3:_="">
     <xsd:import namespace="0fefa867-d15f-4a0d-9945-ea6297accf67"/>
@@ -4502,20 +4564,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7B86EC6-7D1E-4865-AE9C-08032C03144E}"/>
 </file>
</xml_diff>

<commit_message>
Added Microsoft Hackathon Badge
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24722"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24821"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF858760-F757-4B8E-A7CC-3B57758DE4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC511D08-279B-407D-9B36-306EEF2AA2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certifications" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="319">
   <si>
     <t>Title</t>
   </si>
@@ -57,10 +57,19 @@
     <t>IssuedOn</t>
   </si>
   <si>
+    <t>AI ML WORKATHON 2021—Participant</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>9f939e42-85a9-4373-8ea6-9cf7894d856b</t>
+  </si>
+  <si>
+    <t>https://www.credly.com/badges/9f939e42-85a9-4373-8ea6-9cf7894d856b/public_url</t>
+  </si>
+  <si>
     <t>Microsoft Certified: Azure AI Fundamentals</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
   </si>
   <si>
     <t>I045-9367</t>
@@ -1161,7 +1170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1189,7 +1198,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1231,12 +1239,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1552,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1593,50 +1600,47 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="5"/>
+      <c r="G2" s="20">
+        <v>44552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="36">
         <v>0.98</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G3" s="27">
         <v>44527</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D3)</f>
-        <v>https://www.hackerrank.com/certificates/524e499db551</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="20">
-        <v>44493</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1644,209 +1648,209 @@
         <v>14</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="35" t="str">
+      <c r="D4" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="34" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D4)</f>
+        <v>https://www.hackerrank.com/certificates/524e499db551</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21">
+        <v>44493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="34" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D5)</f>
         <v>https://www.hackerrank.com/certificates/7a872682b210</v>
       </c>
-      <c r="F4" s="13">
-        <v>1</v>
-      </c>
-      <c r="G4" s="21">
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21">
         <v>44490</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D5)</f>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D6)</f>
         <v>https://www.hackerrank.com/certificates/eafe133d26dc</v>
       </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="20">
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="20">
         <v>44469</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="26" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="37">
+      <c r="D7" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="36">
         <v>0.94</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G7" s="27">
         <v>44439</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="20">
-        <v>44419</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="34" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="13">
         <v>1</v>
       </c>
       <c r="G8" s="21">
+        <v>44419</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1</v>
+      </c>
+      <c r="G9" s="21">
         <v>44418</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="20">
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
         <v>44418</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="41" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="43">
+      <c r="D11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="36">
         <v>0.88</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G11" s="27">
         <v>44412</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="20">
+    <row r="12" spans="1:7">
+      <c r="A12" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="36">
+        <v>1</v>
+      </c>
+      <c r="G12" s="27">
         <v>44388</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="36" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D12)</f>
-        <v>https://verify.greatlearning.in/UAEGKOSB</v>
-      </c>
-      <c r="F12" s="37">
-        <v>1</v>
-      </c>
-      <c r="G12" s="28">
-        <v>44348</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1857,44 +1861,44 @@
         <v>41</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D13)</f>
-        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D13)</f>
+        <v>https://verify.greatlearning.in/UAEGKOSB</v>
       </c>
       <c r="F13" s="7">
         <v>1</v>
       </c>
       <c r="G13" s="20">
-        <v>44346</v>
+        <v>44348</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D14)</f>
-        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
+        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
       </c>
       <c r="G14" s="20">
-        <v>44339</v>
+        <v>44346</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1905,20 +1909,20 @@
         <v>48</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D15)</f>
-        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
+        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
       </c>
       <c r="F15" s="13">
         <v>1</v>
       </c>
       <c r="G15" s="21">
-        <v>44332</v>
+        <v>44339</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1929,37 +1933,37 @@
         <v>51</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="35" t="s">
-        <v>53</v>
+      <c r="E16" s="34" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D16)</f>
+        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
       </c>
       <c r="F16" s="13">
         <v>1</v>
       </c>
       <c r="G16" s="21">
-        <v>44312</v>
+        <v>44332</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D17)</f>
-        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
+      <c r="E17" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="F17" s="7">
         <v>1</v>
@@ -1970,26 +1974,26 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D18)</f>
-        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
+        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="G18" s="20">
-        <v>44309</v>
+        <v>44312</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2000,44 +2004,44 @@
         <v>60</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D19)</f>
+        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="20">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="35" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D20)</f>
         <v>https://ude.my/UC-1f46a0d1-37f4-4a8c-95f6-839311438ab7</v>
       </c>
-      <c r="F19" s="7">
-        <v>1</v>
-      </c>
-      <c r="G19" s="20">
+      <c r="F20" s="36">
+        <v>1</v>
+      </c>
+      <c r="G20" s="27">
         <v>44306</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="36" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D20)</f>
-        <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
-      </c>
-      <c r="F20" s="37">
-        <v>1</v>
-      </c>
-      <c r="G20" s="28">
-        <v>44300</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2045,41 +2049,41 @@
         <v>65</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D21)</f>
-        <v>https://www.hackerrank.com/certificates/cf58231a440f</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D21)</f>
+        <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
       </c>
       <c r="F21" s="13">
         <v>1</v>
       </c>
       <c r="G21" s="21">
-        <v>44288</v>
+        <v>44300</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="35" t="str">
+        <v>69</v>
+      </c>
+      <c r="E22" s="34" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D22)</f>
-        <v>https://www.hackerrank.com/certificates/4490b4a0e606</v>
+        <v>https://www.hackerrank.com/certificates/cf58231a440f</v>
       </c>
       <c r="F22" s="13">
         <v>1</v>
@@ -2090,20 +2094,20 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" s="6" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D23)</f>
-        <v>https://www.hackerrank.com/certificates/fdeeaad81310</v>
+        <v>https://www.hackerrank.com/certificates/4490b4a0e606</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
@@ -2114,44 +2118,44 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E24" s="6" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D24)</f>
-        <v>https://verify.greatlearning.in/SSMRYOWJ</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D24)</f>
+        <v>https://www.hackerrank.com/certificates/fdeeaad81310</v>
       </c>
       <c r="F24" s="7">
         <v>1</v>
       </c>
       <c r="G24" s="20">
-        <v>44287</v>
+        <v>44288</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E25" s="6" t="str">
         <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D25)</f>
-        <v>https://verify.greatlearning.in/ZYQTXTJA</v>
+        <v>https://verify.greatlearning.in/SSMRYOWJ</v>
       </c>
       <c r="F25" s="7">
         <v>1</v>
@@ -2161,99 +2165,99 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="26" t="s">
+      <c r="A26" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="36" t="str">
+      <c r="B26" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="35" t="str">
         <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D26)</f>
+        <v>https://verify.greatlearning.in/ZYQTXTJA</v>
+      </c>
+      <c r="F26" s="36">
+        <v>1</v>
+      </c>
+      <c r="G26" s="27">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="35" t="str">
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D27)</f>
         <v>https://verify.greatlearning.in/GQGRZFQQ</v>
       </c>
-      <c r="F26" s="37">
-        <v>1</v>
-      </c>
-      <c r="G26" s="28">
-        <v>44287</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="36" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D27)</f>
-        <v>https://verify.greatlearning.in/HSNELKCZ</v>
-      </c>
-      <c r="F27" s="43">
-        <v>1</v>
-      </c>
-      <c r="G27" s="42">
+      <c r="F27" s="42">
+        <v>1</v>
+      </c>
+      <c r="G27" s="41">
         <v>44287</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E28" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D28)</f>
-        <v>https://www.hackerrank.com/certificates/1cadc360a79d</v>
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D28)</f>
+        <v>https://verify.greatlearning.in/HSNELKCZ</v>
       </c>
       <c r="F28" s="13">
         <v>1</v>
       </c>
       <c r="G28" s="21">
-        <v>44268</v>
+        <v>44287</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>83</v>
       </c>
       <c r="E29" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D29)</f>
-        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D29)</f>
+        <v>https://www.hackerrank.com/certificates/1cadc360a79d</v>
       </c>
       <c r="F29" s="13">
         <v>1</v>
       </c>
       <c r="G29" s="20">
-        <v>44249</v>
+        <v>44268</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2264,66 +2268,67 @@
         <v>85</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="35" t="s">
-        <v>87</v>
+      <c r="E30" s="34" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D30)</f>
+        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
       </c>
       <c r="F30" s="13">
-        <v>0.97</v>
-      </c>
-      <c r="G30" s="19">
-        <v>44246</v>
+        <v>1</v>
+      </c>
+      <c r="G30" s="21">
+        <v>44249</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="C31" s="5" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D31)</f>
+      <c r="E31" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.97</v>
+      </c>
+      <c r="G31" s="17">
+        <v>44246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="35" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D32)</f>
         <v>https://www.hackerrank.com/certificates/6730CF1D0F21</v>
       </c>
-      <c r="F31" s="7">
-        <v>1</v>
-      </c>
-      <c r="G31" s="17">
+      <c r="F32" s="36">
+        <v>1</v>
+      </c>
+      <c r="G32" s="44">
         <v>44209</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="37">
-        <v>1</v>
-      </c>
-      <c r="G32" s="47">
-        <v>44180</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2331,117 +2336,116 @@
         <v>93</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="8">
-        <v>271676</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
       <c r="G33" s="17">
-        <v>44176</v>
+        <v>44180</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D34" s="8">
         <v>271676</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
-      <c r="G34" s="20">
+      <c r="G34" s="17">
         <v>44176</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>98</v>
       </c>
       <c r="C35" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="47">
+        <v>271676</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D35)</f>
-        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
-      </c>
       <c r="F35" s="13">
         <v>1</v>
       </c>
-      <c r="G35" s="19">
-        <v>44165</v>
+      <c r="G35" s="21">
+        <v>44176</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>12</v>
-      </c>
       <c r="C36" s="12" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E36" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D36)</f>
-        <v>https://www.hackerrank.com/certificates/3AF4DDB28FAB</v>
+        <v>103</v>
+      </c>
+      <c r="E36" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D36)</f>
+        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
       </c>
       <c r="F36" s="7">
         <v>1</v>
       </c>
       <c r="G36" s="19">
-        <v>44146</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D37)</f>
-        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
+      <c r="E37" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D37)</f>
+        <v>https://www.hackerrank.com/certificates/3AF4DDB28FAB</v>
       </c>
       <c r="F37" s="7">
         <v>1</v>
       </c>
       <c r="G37" s="19">
-        <v>44135</v>
+        <v>44146</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2452,13 +2456,14 @@
         <v>107</v>
       </c>
       <c r="C38" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>110</v>
+      <c r="E38" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D38)</f>
+        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
@@ -2469,44 +2474,43 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E39" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D39)</f>
-        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
+      <c r="E39" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
       </c>
       <c r="G39" s="19">
-        <v>44126</v>
+        <v>44135</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E40" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D40)</f>
-        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
+        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
@@ -2517,20 +2521,20 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E41" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D41)</f>
-        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D41)</f>
+        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
@@ -2541,26 +2545,26 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>119</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D42)</f>
-        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D42)</f>
+        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
       </c>
       <c r="F42" s="16">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G42" s="19">
-        <v>44124</v>
+        <v>44126</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2568,20 +2572,20 @@
         <v>120</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E43" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D43)</f>
-        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D43)</f>
+        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
       </c>
       <c r="F43" s="16">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G43" s="19">
         <v>44124</v>
@@ -2589,47 +2593,47 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E44" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D44)</f>
-        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D44)</f>
+        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
       </c>
       <c r="F44" s="16">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G44" s="19">
-        <v>44122</v>
+        <v>44124</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>126</v>
       </c>
       <c r="E45" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D45)</f>
-        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D45)</f>
+        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
       </c>
       <c r="F45" s="16">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G45" s="19">
         <v>44122</v>
@@ -2643,20 +2647,20 @@
         <v>128</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>129</v>
       </c>
       <c r="E46" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D46)</f>
-        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D46)</f>
+        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
       </c>
       <c r="F46" s="16">
         <v>1</v>
       </c>
       <c r="G46" s="19">
-        <v>44112</v>
+        <v>44122</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2664,41 +2668,41 @@
         <v>130</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E47" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D47)</f>
-        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
+        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
       </c>
       <c r="F47" s="16">
         <v>1</v>
       </c>
       <c r="G47" s="19">
-        <v>44105</v>
+        <v>44112</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E48" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D48)</f>
-        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
+        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
       </c>
       <c r="F48" s="16">
         <v>1</v>
@@ -2709,68 +2713,68 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E49" s="6" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D49)</f>
-        <v>https://verify.greatlearning.in/UYEYVCWB</v>
+        <v>136</v>
+      </c>
+      <c r="E49" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D49)</f>
+        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
       </c>
-      <c r="G49" s="21">
+      <c r="G49" s="19">
         <v>44105</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D50)</f>
-        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
+        <v>137</v>
+      </c>
+      <c r="E50" s="6" t="str">
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D50)</f>
+        <v>https://verify.greatlearning.in/UYEYVCWB</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
       </c>
-      <c r="G50" s="17">
-        <v>44104</v>
+      <c r="G50" s="20">
+        <v>44105</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E51" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D51)</f>
-        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
+        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
       </c>
       <c r="F51" s="7">
         <v>1</v>
@@ -2781,90 +2785,91 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>99</v>
+        <v>128</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E52" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D52)</f>
-        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
+        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
       </c>
       <c r="F52" s="13">
         <v>1</v>
       </c>
       <c r="G52" s="19">
-        <v>44080</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>99</v>
+        <v>107</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E53" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D53)</f>
-        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
+        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
       </c>
       <c r="F53" s="7">
         <v>1</v>
       </c>
-      <c r="G53" s="20">
-        <v>44067</v>
+      <c r="G53" s="17">
+        <v>44080</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D54" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E54" s="6" t="s">
-        <v>145</v>
+      <c r="E54" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D54)</f>
+        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
       </c>
       <c r="F54" s="13">
         <v>1</v>
       </c>
       <c r="G54" s="20">
-        <v>44066</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="C55" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F55" s="13">
         <v>1</v>
@@ -2875,19 +2880,19 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F56" s="13">
         <v>1</v>
@@ -2898,44 +2903,43 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E57" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D57)</f>
-        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
+      <c r="B57" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="F57" s="13">
         <v>1</v>
       </c>
-      <c r="G57" s="17">
-        <v>44063</v>
+      <c r="G57" s="20">
+        <v>44066</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E58" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D58)</f>
-        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D58)</f>
+        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
       </c>
       <c r="F58" s="13">
         <v>1</v>
@@ -2946,212 +2950,212 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>118</v>
+        <v>155</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E59" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D59)</f>
-        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D59)</f>
+        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
       </c>
       <c r="F59" s="7">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G59" s="17">
-        <v>44056</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E60" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D60)</f>
-        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
+        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
       </c>
       <c r="F60" s="7">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="G60" s="17">
-        <v>44055</v>
+        <v>44056</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>42</v>
+        <v>121</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E61" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D61)</f>
+        <v>160</v>
+      </c>
+      <c r="E61" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D61)</f>
+        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
+      </c>
+      <c r="F61" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="G61" s="17">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E62" s="35" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D62)</f>
         <v>https://ude.my/UC-57e2fe2c-3570-4bb3-862f-19b05a9b4413</v>
       </c>
-      <c r="F61" s="7">
-        <v>1</v>
-      </c>
-      <c r="G61" s="17">
+      <c r="F62" s="42">
+        <v>1</v>
+      </c>
+      <c r="G62" s="43">
         <v>44054</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="B62" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="C62" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="D62" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="E62" s="45" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D62)</f>
-        <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
-      </c>
-      <c r="F62" s="43">
-        <v>1</v>
-      </c>
-      <c r="G62" s="44">
-        <v>44022</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E63" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D63)</f>
-        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+        <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
       </c>
       <c r="F63" s="13">
         <v>1</v>
       </c>
       <c r="G63" s="17">
-        <v>44021</v>
+        <v>44022</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E64" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D64)</f>
+        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+      </c>
+      <c r="F64" s="13">
+        <v>1</v>
+      </c>
+      <c r="G64" s="17">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E65" s="10" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D65)</f>
         <v>https://www.coursera.org/verify/L4NCNJMVFQPU</v>
       </c>
-      <c r="F64" s="13">
-        <v>1</v>
-      </c>
-      <c r="G64" s="17">
+      <c r="F65" s="13">
+        <v>1</v>
+      </c>
+      <c r="G65" s="19">
         <v>44013</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E65" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D65)</f>
-        <v>https://www.hackerrank.com/certificates/867DAFFABDA4</v>
-      </c>
-      <c r="F65" s="11">
-        <v>1</v>
-      </c>
-      <c r="G65" s="19">
-        <v>44004</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E66" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D66)</f>
-        <v>https://www.hackerrank.com/certificates/2766975846A6</v>
+        <v>https://www.hackerrank.com/certificates/867DAFFABDA4</v>
       </c>
       <c r="F66" s="11">
         <v>1</v>
       </c>
       <c r="G66" s="19">
-        <v>44003</v>
+        <v>44004</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E67" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D67)</f>
-        <v>https://www.hackerrank.com/certificates/1140C95B9B14</v>
+        <v>https://www.hackerrank.com/certificates/2766975846A6</v>
       </c>
       <c r="F67" s="11">
         <v>1</v>
@@ -3161,75 +3165,75 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="5" t="s">
-        <v>25</v>
+      <c r="A68" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>171</v>
+        <v>15</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="E68" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D68)</f>
-        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
-      </c>
-      <c r="F68" s="13">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D68)</f>
+        <v>https://www.hackerrank.com/certificates/1140C95B9B14</v>
+      </c>
+      <c r="F68" s="11">
         <v>1</v>
       </c>
       <c r="G68" s="17">
-        <v>43999</v>
+        <v>44003</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>99</v>
+        <v>28</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E69" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D69)</f>
-        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
+        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
       </c>
       <c r="F69" s="13">
-        <v>0.94</v>
+        <v>1</v>
       </c>
       <c r="G69" s="17">
-        <v>43995</v>
+        <v>43999</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>175</v>
+        <v>107</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>176</v>
       </c>
       <c r="E70" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D70)</f>
-        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
       </c>
       <c r="F70" s="16">
         <v>0.94</v>
       </c>
       <c r="G70" s="17">
-        <v>43987</v>
+        <v>43995</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3237,46 +3241,47 @@
         <v>177</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E71" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D71)</f>
+        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+      </c>
+      <c r="F71" s="16">
+        <v>0.94</v>
+      </c>
+      <c r="G71" s="17">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E72" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D72)</f>
         <v>https://www.coursera.org/verify/3W45QQBKACKZ</v>
       </c>
-      <c r="F71" s="16">
-        <v>1</v>
-      </c>
-      <c r="G71" s="17">
+      <c r="F72" s="7">
+        <v>1</v>
+      </c>
+      <c r="G72" s="17">
         <v>43986</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F72" s="4">
-        <v>1</v>
-      </c>
-      <c r="G72" s="17">
-        <v>43984</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3284,33 +3289,33 @@
         <v>182</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="E73" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="F73" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G73" s="17">
-        <v>43983</v>
+        <v>43984</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>188</v>
@@ -3319,105 +3324,105 @@
         <v>189</v>
       </c>
       <c r="F74" s="4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G74" s="17">
         <v>43983</v>
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="49" t="s">
+      <c r="A75" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C75" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D75" s="12" t="s">
+      <c r="E75" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="E75" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D75)</f>
-        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
-      </c>
-      <c r="F75" s="13">
-        <v>0.83</v>
+      <c r="F75" s="11">
+        <v>0.8</v>
       </c>
       <c r="G75" s="19">
         <v>43983</v>
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="B76" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D76" s="9" t="s">
+      <c r="B76" s="46" t="s">
         <v>194</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="E76" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D76)</f>
-        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
-      </c>
-      <c r="F76" s="11">
-        <v>1</v>
+        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
+      </c>
+      <c r="F76" s="13">
+        <v>0.83</v>
       </c>
       <c r="G76" s="19">
-        <v>43978</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C77" s="40" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="C77" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E77" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D77)</f>
-        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
+        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
       </c>
       <c r="F77" s="11">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G77" s="19">
-        <v>43968</v>
+        <v>43978</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E78" s="3" t="s">
         <v>199</v>
       </c>
+      <c r="E78" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D78)</f>
+        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
+      </c>
       <c r="F78" s="4">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G78" s="17">
-        <v>43965</v>
+        <v>43968</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3425,56 +3430,56 @@
         <v>200</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="F79" s="4">
         <v>1</v>
       </c>
       <c r="G79" s="17">
-        <v>43956</v>
+        <v>43965</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B80" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="C80" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="E80" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>208</v>
-      </c>
       <c r="F80" s="11">
         <v>1</v>
       </c>
       <c r="G80" s="19">
-        <v>43953</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>210</v>
@@ -3486,7 +3491,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="17">
-        <v>43871</v>
+        <v>43953</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3494,10 +3499,10 @@
         <v>212</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>213</v>
@@ -3509,88 +3514,112 @@
         <v>1</v>
       </c>
       <c r="G82" s="19">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F83" s="11">
+        <v>1</v>
+      </c>
+      <c r="G83" s="19">
         <v>43551</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E83" s="3" t="s">
+    <row r="84" spans="1:7">
+      <c r="A84" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F83" s="4">
-        <v>1</v>
-      </c>
-      <c r="G83" s="17">
+      <c r="B84" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F84" s="4">
+        <v>1</v>
+      </c>
+      <c r="G84" s="17">
         <v>43549</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G83" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G83">
-      <sortCondition descending="1" ref="G1:G83"/>
+  <autoFilter ref="A1:G84" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G84">
+      <sortCondition descending="1" ref="G1:G84"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E83" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
-    <hyperlink ref="E82" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
-    <hyperlink ref="E81" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
-    <hyperlink ref="E79" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
-    <hyperlink ref="E80" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
-    <hyperlink ref="E77" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
-    <hyperlink ref="E78" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
-    <hyperlink ref="E72" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
-    <hyperlink ref="E73" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
-    <hyperlink ref="E74" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
-    <hyperlink ref="E66" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
-    <hyperlink ref="E67" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
-    <hyperlink ref="E65" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
-    <hyperlink ref="E38" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
-    <hyperlink ref="E36" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
-    <hyperlink ref="E33" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
-    <hyperlink ref="E32" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
-    <hyperlink ref="E31" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
-    <hyperlink ref="E30" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
-    <hyperlink ref="E11" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
-    <hyperlink ref="E8" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
-    <hyperlink ref="E9" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
-    <hyperlink ref="E10" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
-    <hyperlink ref="E12" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
-    <hyperlink ref="E16" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
-    <hyperlink ref="E21" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
-    <hyperlink ref="E24" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
-    <hyperlink ref="E25" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
-    <hyperlink ref="E26" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
-    <hyperlink ref="E22" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
-    <hyperlink ref="E23" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
-    <hyperlink ref="E28" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
-    <hyperlink ref="E34" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
-    <hyperlink ref="E54" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
-    <hyperlink ref="E55" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
-    <hyperlink ref="E56" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
-    <hyperlink ref="E7" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
-    <hyperlink ref="E76" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
+    <hyperlink ref="E84" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
+    <hyperlink ref="E83" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
+    <hyperlink ref="E82" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
+    <hyperlink ref="E80" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
+    <hyperlink ref="E81" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
+    <hyperlink ref="E78" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
+    <hyperlink ref="E79" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
+    <hyperlink ref="E73" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
+    <hyperlink ref="E74" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
+    <hyperlink ref="E75" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
+    <hyperlink ref="E67" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
+    <hyperlink ref="E68" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
+    <hyperlink ref="E66" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
+    <hyperlink ref="E39" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
+    <hyperlink ref="E37" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
+    <hyperlink ref="E34" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
+    <hyperlink ref="E33" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
+    <hyperlink ref="E32" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
+    <hyperlink ref="E31" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
+    <hyperlink ref="E12" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
+    <hyperlink ref="E9" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
+    <hyperlink ref="E10" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
+    <hyperlink ref="E11" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
+    <hyperlink ref="E13" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
+    <hyperlink ref="E17" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
+    <hyperlink ref="E22" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
+    <hyperlink ref="E25" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
+    <hyperlink ref="E26" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
+    <hyperlink ref="E27" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
+    <hyperlink ref="E23" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
+    <hyperlink ref="E24" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
+    <hyperlink ref="E29" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
+    <hyperlink ref="E35" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
+    <hyperlink ref="E55" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
+    <hyperlink ref="E56" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
+    <hyperlink ref="E57" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
+    <hyperlink ref="E8" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
+    <hyperlink ref="E77" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
     <hyperlink ref="E29:E42" r:id="rId39" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{CE0B26B0-E940-4BD5-8F74-8D28A4F3B13A}"/>
-    <hyperlink ref="E35" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
-    <hyperlink ref="E53" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
-    <hyperlink ref="E13" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
+    <hyperlink ref="E36" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
+    <hyperlink ref="E54" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
+    <hyperlink ref="E14" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
     <hyperlink ref="E9:E10" r:id="rId43" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{C55AB7BE-0BE1-4CE1-8CFE-C0E7B2B0BA28}"/>
     <hyperlink ref="E12:E15" r:id="rId44" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{549C4CBA-43AF-4870-BE36-8D1CBC3CFD71}"/>
-    <hyperlink ref="E29" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
-    <hyperlink ref="E61" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
-    <hyperlink ref="E6" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
-    <hyperlink ref="E5" r:id="rId48" display="https://www.hackerrank.com/certificates/eafe133d26dc" xr:uid="{3748E750-A80A-4402-BC5F-803B16F27441}"/>
-    <hyperlink ref="E2" r:id="rId49" xr:uid="{59D89928-3553-4495-8CD7-92EBC3B422E3}"/>
+    <hyperlink ref="E30" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
+    <hyperlink ref="E62" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
+    <hyperlink ref="E7" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
+    <hyperlink ref="E6" r:id="rId48" display="https://www.hackerrank.com/certificates/eafe133d26dc" xr:uid="{3748E750-A80A-4402-BC5F-803B16F27441}"/>
+    <hyperlink ref="E3" r:id="rId49" xr:uid="{59D89928-3553-4495-8CD7-92EBC3B422E3}"/>
+    <hyperlink ref="E2" r:id="rId50" xr:uid="{90A10946-4B5C-4200-83CE-B2047CBD914F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3618,27 +3647,27 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>224</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="G1" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="E1" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -3647,73 +3676,73 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="28">
+      <c r="C2" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2" s="27">
         <v>44470</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>230</v>
+      <c r="G2" s="27" t="s">
+        <v>233</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" s="27">
+        <v>44378</v>
+      </c>
+      <c r="G3" s="27">
+        <v>44469</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="F3" s="28">
-        <v>44378</v>
-      </c>
-      <c r="G3" s="28">
-        <v>44469</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>231</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>234</v>
+        <v>238</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>237</v>
       </c>
       <c r="F4" s="20">
         <v>44263</v>
@@ -3722,54 +3751,54 @@
         <v>44377</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" s="34" customFormat="1" ht="75">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:9" s="33" customFormat="1" ht="75">
+      <c r="A5" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>237</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>239</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="E5" s="31" t="s">
+      <c r="F5" s="31">
+        <v>44137</v>
+      </c>
+      <c r="G5" s="31">
+        <v>44200</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="F5" s="32">
-        <v>44137</v>
-      </c>
-      <c r="G5" s="32">
-        <v>44200</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>240</v>
+      <c r="I5" s="32" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>234</v>
+        <v>245</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>237</v>
       </c>
       <c r="F6" s="20">
         <v>44136</v>
@@ -3778,27 +3807,27 @@
         <v>44166</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>234</v>
+      <c r="C7" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>237</v>
       </c>
       <c r="F7" s="20">
         <v>44105</v>
@@ -3807,27 +3836,27 @@
         <v>44136</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>234</v>
+        <v>253</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>237</v>
       </c>
       <c r="F8" s="20">
         <v>43432</v>
@@ -3836,10 +3865,10 @@
         <v>43442</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3906,7 +3935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718451B2-E12D-4ABD-B26C-5975AED3964E}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3915,16 +3944,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>253</v>
+      <c r="A1" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B2" s="7">
         <v>0.9</v>
@@ -3932,7 +3961,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B3" s="7">
         <v>0.8</v>
@@ -3940,7 +3969,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B4" s="7">
         <v>0.8</v>
@@ -3948,7 +3977,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B5" s="7">
         <v>0.8</v>
@@ -3956,7 +3985,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B6" s="7">
         <v>0.8</v>
@@ -3964,7 +3993,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B7" s="7">
         <v>0.8</v>
@@ -3972,7 +4001,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B8" s="7">
         <v>0.8</v>
@@ -3980,7 +4009,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B9" s="7">
         <v>0.7</v>
@@ -3988,7 +4017,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B10" s="7">
         <v>0.7</v>
@@ -3996,7 +4025,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B11" s="7">
         <v>0.7</v>
@@ -4004,7 +4033,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B12" s="7">
         <v>0.7</v>
@@ -4012,7 +4041,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B13" s="7">
         <v>0.6</v>
@@ -4020,7 +4049,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B14" s="7">
         <v>0.6</v>
@@ -4028,7 +4057,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B15" s="7">
         <v>0.6</v>
@@ -4036,7 +4065,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B16" s="7">
         <v>0.6</v>
@@ -4044,7 +4073,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B17" s="7">
         <v>0.6</v>
@@ -4052,7 +4081,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B18" s="7">
         <v>0.6</v>
@@ -4060,7 +4089,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B19" s="7">
         <v>0.6</v>
@@ -4068,7 +4097,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B20" s="7">
         <v>0.5</v>
@@ -4076,7 +4105,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B21" s="7">
         <v>0.5</v>
@@ -4084,7 +4113,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B22" s="7">
         <v>0.5</v>
@@ -4117,199 +4146,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>274</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>275</v>
+      <c r="B1" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -4333,18 +4362,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4565,11 +4594,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Reset to previous commits
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24722"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24821"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF858760-F757-4B8E-A7CC-3B57758DE4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7F9B1D1-5E01-499D-B3BB-20F64BE914BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certifications" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="319">
   <si>
     <t>Title</t>
   </si>
@@ -57,10 +57,19 @@
     <t>IssuedOn</t>
   </si>
   <si>
+    <t>AI ML WORKATHON 2021—Participant</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>9f939e42-85a9-4373-8ea6-9cf7894d856b</t>
+  </si>
+  <si>
+    <t>https://www.credly.com/badges/9f939e42-85a9-4373-8ea6-9cf7894d856b/public_url</t>
+  </si>
+  <si>
     <t>Microsoft Certified: Azure AI Fundamentals</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
   </si>
   <si>
     <t>I045-9367</t>
@@ -1161,7 +1170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1189,7 +1198,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1231,12 +1239,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1552,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1593,50 +1600,49 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20">
+        <v>44552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="36">
         <v>0.98</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G3" s="27">
         <v>44527</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D3)</f>
-        <v>https://www.hackerrank.com/certificates/524e499db551</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="20">
-        <v>44493</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1644,209 +1650,209 @@
         <v>14</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="35" t="str">
+      <c r="D4" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="34" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D4)</f>
+        <v>https://www.hackerrank.com/certificates/524e499db551</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21">
+        <v>44493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="34" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D5)</f>
         <v>https://www.hackerrank.com/certificates/7a872682b210</v>
       </c>
-      <c r="F4" s="13">
-        <v>1</v>
-      </c>
-      <c r="G4" s="21">
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21">
         <v>44490</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D5)</f>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D6)</f>
         <v>https://www.hackerrank.com/certificates/eafe133d26dc</v>
       </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="20">
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="20">
         <v>44469</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="26" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="37">
+      <c r="D7" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="36">
         <v>0.94</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G7" s="27">
         <v>44439</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="20">
-        <v>44419</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="34" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="13">
         <v>1</v>
       </c>
       <c r="G8" s="21">
+        <v>44419</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1</v>
+      </c>
+      <c r="G9" s="21">
         <v>44418</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="20">
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
         <v>44418</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="41" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="43">
+      <c r="D11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="36">
         <v>0.88</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G11" s="27">
         <v>44412</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="20">
+    <row r="12" spans="1:7">
+      <c r="A12" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="36">
+        <v>1</v>
+      </c>
+      <c r="G12" s="27">
         <v>44388</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="36" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D12)</f>
-        <v>https://verify.greatlearning.in/UAEGKOSB</v>
-      </c>
-      <c r="F12" s="37">
-        <v>1</v>
-      </c>
-      <c r="G12" s="28">
-        <v>44348</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1857,44 +1863,44 @@
         <v>41</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D13)</f>
-        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D13)</f>
+        <v>https://verify.greatlearning.in/UAEGKOSB</v>
       </c>
       <c r="F13" s="7">
         <v>1</v>
       </c>
       <c r="G13" s="20">
-        <v>44346</v>
+        <v>44348</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D14)</f>
-        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
+        <v>https://ude.my/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707</v>
       </c>
       <c r="F14" s="7">
         <v>1</v>
       </c>
       <c r="G14" s="20">
-        <v>44339</v>
+        <v>44346</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1905,20 +1911,20 @@
         <v>48</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D15)</f>
-        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
+        <v>https://ude.my/UC-a3ba46b5-170d-4510-a813-c3dff69a6697</v>
       </c>
       <c r="F15" s="13">
         <v>1</v>
       </c>
       <c r="G15" s="21">
-        <v>44332</v>
+        <v>44339</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1929,37 +1935,37 @@
         <v>51</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="35" t="s">
-        <v>53</v>
+      <c r="E16" s="34" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D16)</f>
+        <v>https://ude.my/UC-6ee1aa7b-93ad-4437-ac78-fb96957a2f3b</v>
       </c>
       <c r="F16" s="13">
         <v>1</v>
       </c>
       <c r="G16" s="21">
-        <v>44312</v>
+        <v>44332</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D17)</f>
-        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
+      <c r="E17" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="F17" s="7">
         <v>1</v>
@@ -1970,26 +1976,26 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D18)</f>
-        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
+        <v>https://ude.my/UC-c9ca1de5-ac7a-449c-923d-aa727cbd1906</v>
       </c>
       <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="G18" s="20">
-        <v>44309</v>
+        <v>44312</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2000,44 +2006,44 @@
         <v>60</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="6" t="str">
         <f>HYPERLINK("https://ude.my/"&amp; D19)</f>
+        <v>https://ude.my/UC-b2d528a0-beba-44fc-96bb-c1ccd88ee68a</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="20">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="35" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D20)</f>
         <v>https://ude.my/UC-1f46a0d1-37f4-4a8c-95f6-839311438ab7</v>
       </c>
-      <c r="F19" s="7">
-        <v>1</v>
-      </c>
-      <c r="G19" s="20">
+      <c r="F20" s="36">
+        <v>1</v>
+      </c>
+      <c r="G20" s="27">
         <v>44306</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="36" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D20)</f>
-        <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
-      </c>
-      <c r="F20" s="37">
-        <v>1</v>
-      </c>
-      <c r="G20" s="28">
-        <v>44300</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2045,41 +2051,41 @@
         <v>65</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D21)</f>
-        <v>https://www.hackerrank.com/certificates/cf58231a440f</v>
+        <f>HYPERLINK("https://ude.my/"&amp; D21)</f>
+        <v>https://ude.my/UC-18dd832f-d345-44f1-92cf-281f71e773d1</v>
       </c>
       <c r="F21" s="13">
         <v>1</v>
       </c>
       <c r="G21" s="21">
-        <v>44288</v>
+        <v>44300</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="35" t="str">
+        <v>69</v>
+      </c>
+      <c r="E22" s="34" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D22)</f>
-        <v>https://www.hackerrank.com/certificates/4490b4a0e606</v>
+        <v>https://www.hackerrank.com/certificates/cf58231a440f</v>
       </c>
       <c r="F22" s="13">
         <v>1</v>
@@ -2090,20 +2096,20 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" s="6" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D23)</f>
-        <v>https://www.hackerrank.com/certificates/fdeeaad81310</v>
+        <v>https://www.hackerrank.com/certificates/4490b4a0e606</v>
       </c>
       <c r="F23" s="7">
         <v>1</v>
@@ -2114,44 +2120,44 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E24" s="6" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D24)</f>
-        <v>https://verify.greatlearning.in/SSMRYOWJ</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D24)</f>
+        <v>https://www.hackerrank.com/certificates/fdeeaad81310</v>
       </c>
       <c r="F24" s="7">
         <v>1</v>
       </c>
       <c r="G24" s="20">
-        <v>44287</v>
+        <v>44288</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E25" s="6" t="str">
         <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D25)</f>
-        <v>https://verify.greatlearning.in/ZYQTXTJA</v>
+        <v>https://verify.greatlearning.in/SSMRYOWJ</v>
       </c>
       <c r="F25" s="7">
         <v>1</v>
@@ -2161,99 +2167,99 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="26" t="s">
+      <c r="A26" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="36" t="str">
+      <c r="B26" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="35" t="str">
         <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D26)</f>
+        <v>https://verify.greatlearning.in/ZYQTXTJA</v>
+      </c>
+      <c r="F26" s="36">
+        <v>1</v>
+      </c>
+      <c r="G26" s="27">
+        <v>44287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="35" t="str">
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D27)</f>
         <v>https://verify.greatlearning.in/GQGRZFQQ</v>
       </c>
-      <c r="F26" s="37">
-        <v>1</v>
-      </c>
-      <c r="G26" s="28">
-        <v>44287</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="36" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D27)</f>
-        <v>https://verify.greatlearning.in/HSNELKCZ</v>
-      </c>
-      <c r="F27" s="43">
-        <v>1</v>
-      </c>
-      <c r="G27" s="42">
+      <c r="F27" s="42">
+        <v>1</v>
+      </c>
+      <c r="G27" s="41">
         <v>44287</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E28" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D28)</f>
-        <v>https://www.hackerrank.com/certificates/1cadc360a79d</v>
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D28)</f>
+        <v>https://verify.greatlearning.in/HSNELKCZ</v>
       </c>
       <c r="F28" s="13">
         <v>1</v>
       </c>
       <c r="G28" s="21">
-        <v>44268</v>
+        <v>44287</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>83</v>
       </c>
       <c r="E29" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D29)</f>
-        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D29)</f>
+        <v>https://www.hackerrank.com/certificates/1cadc360a79d</v>
       </c>
       <c r="F29" s="13">
         <v>1</v>
       </c>
       <c r="G29" s="20">
-        <v>44249</v>
+        <v>44268</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2264,66 +2270,67 @@
         <v>85</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="35" t="s">
-        <v>87</v>
+      <c r="E30" s="34" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D30)</f>
+        <v>https://ude.my/UC-61e2521b-a9bb-48dc-bb44-3679ba047cf8</v>
       </c>
       <c r="F30" s="13">
-        <v>0.97</v>
-      </c>
-      <c r="G30" s="19">
-        <v>44246</v>
+        <v>1</v>
+      </c>
+      <c r="G30" s="21">
+        <v>44249</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="C31" s="5" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D31)</f>
+      <c r="E31" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.97</v>
+      </c>
+      <c r="G31" s="17">
+        <v>44246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="35" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D32)</f>
         <v>https://www.hackerrank.com/certificates/6730CF1D0F21</v>
       </c>
-      <c r="F31" s="7">
-        <v>1</v>
-      </c>
-      <c r="G31" s="17">
+      <c r="F32" s="36">
+        <v>1</v>
+      </c>
+      <c r="G32" s="44">
         <v>44209</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="37">
-        <v>1</v>
-      </c>
-      <c r="G32" s="47">
-        <v>44180</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2331,117 +2338,116 @@
         <v>93</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="8">
-        <v>271676</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="F33" s="7">
         <v>1</v>
       </c>
       <c r="G33" s="17">
-        <v>44176</v>
+        <v>44180</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D34" s="8">
         <v>271676</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F34" s="7">
         <v>1</v>
       </c>
-      <c r="G34" s="20">
+      <c r="G34" s="17">
         <v>44176</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>98</v>
       </c>
       <c r="C35" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="47">
+        <v>271676</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D35)</f>
-        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
-      </c>
       <c r="F35" s="13">
         <v>1</v>
       </c>
-      <c r="G35" s="19">
-        <v>44165</v>
+      <c r="G35" s="21">
+        <v>44176</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>12</v>
-      </c>
       <c r="C36" s="12" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E36" s="6" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D36)</f>
-        <v>https://www.hackerrank.com/certificates/3AF4DDB28FAB</v>
+        <v>103</v>
+      </c>
+      <c r="E36" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D36)</f>
+        <v>https://www.coursera.org/verify/3NB72YUYKWLV</v>
       </c>
       <c r="F36" s="7">
         <v>1</v>
       </c>
       <c r="G36" s="19">
-        <v>44146</v>
+        <v>44165</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D37)</f>
-        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
+      <c r="E37" s="6" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D37)</f>
+        <v>https://www.hackerrank.com/certificates/3AF4DDB28FAB</v>
       </c>
       <c r="F37" s="7">
         <v>1</v>
       </c>
       <c r="G37" s="19">
-        <v>44135</v>
+        <v>44146</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2452,13 +2458,14 @@
         <v>107</v>
       </c>
       <c r="C38" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>110</v>
+      <c r="E38" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D38)</f>
+        <v>https://www.coursera.org/verify/AW6A4NWBVJ9V</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
@@ -2469,44 +2476,43 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E39" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D39)</f>
-        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
+      <c r="E39" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
       </c>
       <c r="G39" s="19">
-        <v>44126</v>
+        <v>44135</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E40" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D40)</f>
-        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
+        <v>https://www.coursera.org/verify/3WQ6APAJLP9T</v>
       </c>
       <c r="F40" s="7">
         <v>1</v>
@@ -2517,20 +2523,20 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E41" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D41)</f>
-        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D41)</f>
+        <v>https://www.coursera.org/verify/8DZVQYMNERJA</v>
       </c>
       <c r="F41" s="7">
         <v>1</v>
@@ -2541,26 +2547,26 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>119</v>
       </c>
       <c r="E42" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D42)</f>
-        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D42)</f>
+        <v>https://www.coursera.org/verify/specialization/LGGYURMTBUUG</v>
       </c>
       <c r="F42" s="16">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G42" s="19">
-        <v>44124</v>
+        <v>44126</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2568,20 +2574,20 @@
         <v>120</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E43" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D43)</f>
-        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D43)</f>
+        <v>https://www.coursera.org/verify/LVBJNAL79BLV</v>
       </c>
       <c r="F43" s="16">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="G43" s="19">
         <v>44124</v>
@@ -2589,47 +2595,47 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E44" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D44)</f>
-        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D44)</f>
+        <v>https://www.coursera.org/verify/specialization/6NXPUFTEK3Z7</v>
       </c>
       <c r="F44" s="16">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G44" s="19">
-        <v>44122</v>
+        <v>44124</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>126</v>
       </c>
       <c r="E45" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D45)</f>
-        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D45)</f>
+        <v>https://www.coursera.org/verify/4XRSLQYDGXHF</v>
       </c>
       <c r="F45" s="16">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G45" s="19">
         <v>44122</v>
@@ -2643,20 +2649,20 @@
         <v>128</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>129</v>
       </c>
       <c r="E46" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D46)</f>
-        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/account/accomplishments/certificate/" &amp; D46)</f>
+        <v>https://www.coursera.org/account/accomplishments/certificate/6KQ8S8U4FGQ5</v>
       </c>
       <c r="F46" s="16">
         <v>1</v>
       </c>
       <c r="G46" s="19">
-        <v>44112</v>
+        <v>44122</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -2664,41 +2670,41 @@
         <v>130</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E47" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D47)</f>
-        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
+        <v>https://www.coursera.org/verify/7JKY6ZQ9D76M</v>
       </c>
       <c r="F47" s="16">
         <v>1</v>
       </c>
       <c r="G47" s="19">
-        <v>44105</v>
+        <v>44112</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E48" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D48)</f>
-        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
+        <v>https://www.coursera.org/verify/QWX8PHM4TZUF</v>
       </c>
       <c r="F48" s="16">
         <v>1</v>
@@ -2709,68 +2715,68 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E49" s="6" t="str">
-        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D49)</f>
-        <v>https://verify.greatlearning.in/UYEYVCWB</v>
+        <v>136</v>
+      </c>
+      <c r="E49" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D49)</f>
+        <v>https://www.coursera.org/verify/ARXP6JVNYNAM</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
       </c>
-      <c r="G49" s="21">
+      <c r="G49" s="19">
         <v>44105</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D50)</f>
-        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
+        <v>137</v>
+      </c>
+      <c r="E50" s="6" t="str">
+        <f>HYPERLINK("https://verify.greatlearning.in/"&amp;D50)</f>
+        <v>https://verify.greatlearning.in/UYEYVCWB</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
       </c>
-      <c r="G50" s="17">
-        <v>44104</v>
+      <c r="G50" s="20">
+        <v>44105</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E51" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D51)</f>
-        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
+        <v>https://www.coursera.org/verify/EUKYBKW2SUXX</v>
       </c>
       <c r="F51" s="7">
         <v>1</v>
@@ -2781,90 +2787,91 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>99</v>
+        <v>128</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E52" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D52)</f>
-        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
+        <v>https://www.coursera.org/verify/EUTL7GRT9ZQ4</v>
       </c>
       <c r="F52" s="13">
         <v>1</v>
       </c>
       <c r="G52" s="19">
-        <v>44080</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>99</v>
+        <v>107</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E53" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D53)</f>
-        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
+        <v>https://www.coursera.org/verify/MX93X95TXB9V</v>
       </c>
       <c r="F53" s="7">
         <v>1</v>
       </c>
-      <c r="G53" s="20">
-        <v>44067</v>
+      <c r="G53" s="17">
+        <v>44080</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D54" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E54" s="6" t="s">
-        <v>145</v>
+      <c r="E54" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D54)</f>
+        <v>https://www.coursera.org/verify/ERVJF5JMFDRV</v>
       </c>
       <c r="F54" s="13">
         <v>1</v>
       </c>
       <c r="G54" s="20">
-        <v>44066</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="C55" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F55" s="13">
         <v>1</v>
@@ -2875,19 +2882,19 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F56" s="13">
         <v>1</v>
@@ -2898,44 +2905,43 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E57" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D57)</f>
-        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
+      <c r="B57" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="F57" s="13">
         <v>1</v>
       </c>
-      <c r="G57" s="17">
-        <v>44063</v>
+      <c r="G57" s="20">
+        <v>44066</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E58" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D58)</f>
-        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D58)</f>
+        <v>https://www.coursera.org/verify/P53AV7SZHJ52</v>
       </c>
       <c r="F58" s="13">
         <v>1</v>
@@ -2946,212 +2952,212 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>118</v>
+        <v>155</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E59" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D59)</f>
-        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/specialization/" &amp; D59)</f>
+        <v>https://www.coursera.org/verify/specialization/FQXP3E6NT3YM</v>
       </c>
       <c r="F59" s="7">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="G59" s="17">
-        <v>44056</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E60" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D60)</f>
-        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
+        <v>https://www.coursera.org/verify/MQ4NMBLXN3G6</v>
       </c>
       <c r="F60" s="7">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="G60" s="17">
-        <v>44055</v>
+        <v>44056</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>42</v>
+        <v>121</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E61" s="6" t="str">
-        <f>HYPERLINK("https://ude.my/"&amp; D61)</f>
+        <v>160</v>
+      </c>
+      <c r="E61" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D61)</f>
+        <v>https://www.coursera.org/verify/UQ5RQLWBRLJA</v>
+      </c>
+      <c r="F61" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="G61" s="17">
+        <v>44055</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E62" s="35" t="str">
+        <f>HYPERLINK("https://ude.my/"&amp; D62)</f>
         <v>https://ude.my/UC-57e2fe2c-3570-4bb3-862f-19b05a9b4413</v>
       </c>
-      <c r="F61" s="7">
-        <v>1</v>
-      </c>
-      <c r="G61" s="17">
+      <c r="F62" s="42">
+        <v>1</v>
+      </c>
+      <c r="G62" s="43">
         <v>44054</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="B62" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="C62" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="D62" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="E62" s="45" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D62)</f>
-        <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
-      </c>
-      <c r="F62" s="43">
-        <v>1</v>
-      </c>
-      <c r="G62" s="44">
-        <v>44022</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E63" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D63)</f>
-        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+        <v>https://www.coursera.org/verify/HS9S3MQ9U8G5</v>
       </c>
       <c r="F63" s="13">
         <v>1</v>
       </c>
       <c r="G63" s="17">
-        <v>44021</v>
+        <v>44022</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E64" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D64)</f>
+        <v>https://www.coursera.org/verify/Z27MPBY34D3J</v>
+      </c>
+      <c r="F64" s="13">
+        <v>1</v>
+      </c>
+      <c r="G64" s="17">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E65" s="10" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D65)</f>
         <v>https://www.coursera.org/verify/L4NCNJMVFQPU</v>
       </c>
-      <c r="F64" s="13">
-        <v>1</v>
-      </c>
-      <c r="G64" s="17">
+      <c r="F65" s="13">
+        <v>1</v>
+      </c>
+      <c r="G65" s="19">
         <v>44013</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E65" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D65)</f>
-        <v>https://www.hackerrank.com/certificates/867DAFFABDA4</v>
-      </c>
-      <c r="F65" s="11">
-        <v>1</v>
-      </c>
-      <c r="G65" s="19">
-        <v>44004</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E66" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D66)</f>
-        <v>https://www.hackerrank.com/certificates/2766975846A6</v>
+        <v>https://www.hackerrank.com/certificates/867DAFFABDA4</v>
       </c>
       <c r="F66" s="11">
         <v>1</v>
       </c>
       <c r="G66" s="19">
-        <v>44003</v>
+        <v>44004</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E67" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D67)</f>
-        <v>https://www.hackerrank.com/certificates/1140C95B9B14</v>
+        <v>https://www.hackerrank.com/certificates/2766975846A6</v>
       </c>
       <c r="F67" s="11">
         <v>1</v>
@@ -3161,75 +3167,75 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="5" t="s">
-        <v>25</v>
+      <c r="A68" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>171</v>
+        <v>15</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="E68" s="3" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D68)</f>
-        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
-      </c>
-      <c r="F68" s="13">
+        <f xml:space="preserve"> HYPERLINK("https://www.hackerrank.com/certificates/" &amp; D68)</f>
+        <v>https://www.hackerrank.com/certificates/1140C95B9B14</v>
+      </c>
+      <c r="F68" s="11">
         <v>1</v>
       </c>
       <c r="G68" s="17">
-        <v>43999</v>
+        <v>44003</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>99</v>
+        <v>28</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E69" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D69)</f>
-        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
+        <v>https://www.coursera.org/verify/WG7CRBWGK8FW</v>
       </c>
       <c r="F69" s="13">
-        <v>0.94</v>
+        <v>1</v>
       </c>
       <c r="G69" s="17">
-        <v>43995</v>
+        <v>43999</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>175</v>
+        <v>107</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>176</v>
       </c>
       <c r="E70" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D70)</f>
-        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+        <v>https://www.coursera.org/verify/L5XQHDFRBG5S</v>
       </c>
       <c r="F70" s="16">
         <v>0.94</v>
       </c>
       <c r="G70" s="17">
-        <v>43987</v>
+        <v>43995</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3237,46 +3243,47 @@
         <v>177</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>125</v>
+        <v>178</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E71" s="3" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D71)</f>
+        <v>https://www.coursera.org/verify/F6ASNEAAYVGZ</v>
+      </c>
+      <c r="F71" s="16">
+        <v>0.94</v>
+      </c>
+      <c r="G71" s="17">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E72" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D72)</f>
         <v>https://www.coursera.org/verify/3W45QQBKACKZ</v>
       </c>
-      <c r="F71" s="16">
-        <v>1</v>
-      </c>
-      <c r="G71" s="17">
+      <c r="F72" s="7">
+        <v>1</v>
+      </c>
+      <c r="G72" s="17">
         <v>43986</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F72" s="4">
-        <v>1</v>
-      </c>
-      <c r="G72" s="17">
-        <v>43984</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3284,33 +3291,33 @@
         <v>182</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="E73" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="F73" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G73" s="17">
-        <v>43983</v>
+        <v>43984</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>188</v>
@@ -3319,105 +3326,105 @@
         <v>189</v>
       </c>
       <c r="F74" s="4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G74" s="17">
         <v>43983</v>
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="49" t="s">
+      <c r="A75" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C75" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D75" s="12" t="s">
+      <c r="E75" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="E75" s="10" t="str">
-        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D75)</f>
-        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
-      </c>
-      <c r="F75" s="13">
-        <v>0.83</v>
+      <c r="F75" s="11">
+        <v>0.8</v>
       </c>
       <c r="G75" s="19">
         <v>43983</v>
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="B76" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D76" s="9" t="s">
+      <c r="B76" s="46" t="s">
         <v>194</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="E76" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D76)</f>
-        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
-      </c>
-      <c r="F76" s="11">
-        <v>1</v>
+        <v>https://www.coursera.org/verify/ZM9BMYXLN942</v>
+      </c>
+      <c r="F76" s="13">
+        <v>0.83</v>
       </c>
       <c r="G76" s="19">
-        <v>43978</v>
+        <v>43983</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C77" s="40" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="C77" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E77" s="10" t="str">
         <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D77)</f>
-        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
+        <v>https://www.coursera.org/verify/FKLHXG2L7ZV2</v>
       </c>
       <c r="F77" s="11">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G77" s="19">
-        <v>43968</v>
+        <v>43978</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E78" s="3" t="s">
         <v>199</v>
       </c>
+      <c r="E78" s="3" t="str">
+        <f xml:space="preserve"> HYPERLINK("https://www.coursera.org/verify/" &amp; D78)</f>
+        <v>https://www.coursera.org/verify/LSGX9WZD2829</v>
+      </c>
       <c r="F78" s="4">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G78" s="17">
-        <v>43965</v>
+        <v>43968</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3425,56 +3432,56 @@
         <v>200</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="F79" s="4">
         <v>1</v>
       </c>
       <c r="G79" s="17">
-        <v>43956</v>
+        <v>43965</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B80" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="C80" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="E80" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>208</v>
-      </c>
       <c r="F80" s="11">
         <v>1</v>
       </c>
       <c r="G80" s="19">
-        <v>43953</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>210</v>
@@ -3486,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="17">
-        <v>43871</v>
+        <v>43953</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3494,10 +3501,10 @@
         <v>212</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>213</v>
@@ -3509,88 +3516,112 @@
         <v>1</v>
       </c>
       <c r="G82" s="19">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F83" s="11">
+        <v>1</v>
+      </c>
+      <c r="G83" s="19">
         <v>43551</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E83" s="3" t="s">
+    <row r="84" spans="1:7">
+      <c r="A84" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F83" s="4">
-        <v>1</v>
-      </c>
-      <c r="G83" s="17">
+      <c r="B84" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F84" s="4">
+        <v>1</v>
+      </c>
+      <c r="G84" s="17">
         <v>43549</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G83" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G83">
-      <sortCondition descending="1" ref="G1:G83"/>
+  <autoFilter ref="A1:G84" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G84">
+      <sortCondition descending="1" ref="G1:G84"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E83" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
-    <hyperlink ref="E82" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
-    <hyperlink ref="E81" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
-    <hyperlink ref="E79" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
-    <hyperlink ref="E80" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
-    <hyperlink ref="E77" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
-    <hyperlink ref="E78" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
-    <hyperlink ref="E72" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
-    <hyperlink ref="E73" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
-    <hyperlink ref="E74" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
-    <hyperlink ref="E66" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
-    <hyperlink ref="E67" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
-    <hyperlink ref="E65" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
-    <hyperlink ref="E38" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
-    <hyperlink ref="E36" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
-    <hyperlink ref="E33" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
-    <hyperlink ref="E32" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
-    <hyperlink ref="E31" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
-    <hyperlink ref="E30" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
-    <hyperlink ref="E11" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
-    <hyperlink ref="E8" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
-    <hyperlink ref="E9" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
-    <hyperlink ref="E10" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
-    <hyperlink ref="E12" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
-    <hyperlink ref="E16" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
-    <hyperlink ref="E21" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
-    <hyperlink ref="E24" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
-    <hyperlink ref="E25" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
-    <hyperlink ref="E26" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
-    <hyperlink ref="E22" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
-    <hyperlink ref="E23" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
-    <hyperlink ref="E28" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
-    <hyperlink ref="E34" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
-    <hyperlink ref="E54" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
-    <hyperlink ref="E55" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
-    <hyperlink ref="E56" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
-    <hyperlink ref="E7" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
-    <hyperlink ref="E76" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
+    <hyperlink ref="E84" r:id="rId1" xr:uid="{6C0DBD8A-06FB-4276-97CC-44F7D2A620D3}"/>
+    <hyperlink ref="E83" r:id="rId2" xr:uid="{A3AA2B4E-A070-4264-BAD0-50B1BD9F111B}"/>
+    <hyperlink ref="E82" r:id="rId3" xr:uid="{9B48E280-22D3-4A9E-8D60-7F69F560315A}"/>
+    <hyperlink ref="E80" r:id="rId4" xr:uid="{A1888FFC-F836-43B1-ACCE-D7ED9F0B270F}"/>
+    <hyperlink ref="E81" r:id="rId5" xr:uid="{1D430177-A56E-4567-8FAC-5E8420D918CC}"/>
+    <hyperlink ref="E78" r:id="rId6" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{1F5AE59F-A263-4228-9C7E-266BAD69AD6D}"/>
+    <hyperlink ref="E79" r:id="rId7" xr:uid="{CE2198E5-2DEE-4B00-8F0C-17EA31FD42CF}"/>
+    <hyperlink ref="E73" r:id="rId8" xr:uid="{D9C0C981-CB38-4235-A77B-7B73A8D1355B}"/>
+    <hyperlink ref="E74" r:id="rId9" xr:uid="{256B4442-C33A-484D-A51A-03B0A68C0D1A}"/>
+    <hyperlink ref="E75" r:id="rId10" xr:uid="{11511F3E-24A6-40DC-8710-D6F763ABC7D0}"/>
+    <hyperlink ref="E67" r:id="rId11" xr:uid="{23538072-30C4-4325-A871-9979C940114B}"/>
+    <hyperlink ref="E68" r:id="rId12" xr:uid="{92658253-7FDE-4177-9BB5-57ABBEC11707}"/>
+    <hyperlink ref="E66" r:id="rId13" xr:uid="{760F6237-ED74-4C76-921F-A92DB49AA851}"/>
+    <hyperlink ref="E39" r:id="rId14" xr:uid="{BE109821-CCDD-4A04-981A-9F6EFC5839F3}"/>
+    <hyperlink ref="E37" r:id="rId15" xr:uid="{193C03FB-8BC6-4219-AB14-ECE3411E93FC}"/>
+    <hyperlink ref="E34" r:id="rId16" xr:uid="{C4C48324-FD2D-4D60-97F7-1C543194CDA1}"/>
+    <hyperlink ref="E33" r:id="rId17" xr:uid="{24CD5469-5A68-4595-8905-E3195BAA26D6}"/>
+    <hyperlink ref="E32" r:id="rId18" xr:uid="{4E5A9F5D-377D-4813-82DA-653909A03F55}"/>
+    <hyperlink ref="E31" r:id="rId19" xr:uid="{13330E2D-247C-4D68-B3A4-25AEC2481299}"/>
+    <hyperlink ref="E12" r:id="rId20" xr:uid="{104CE576-4E8E-4A67-852D-469446BC152A}"/>
+    <hyperlink ref="E9" r:id="rId21" xr:uid="{F5B1676B-40C2-41E4-8A7C-EE0DDF96B5AB}"/>
+    <hyperlink ref="E10" r:id="rId22" xr:uid="{CF1353C0-1B68-45EB-B9D3-B3815B4819F9}"/>
+    <hyperlink ref="E11" r:id="rId23" xr:uid="{C08302DF-FF6D-47C0-8C56-3AB13A011040}"/>
+    <hyperlink ref="E13" r:id="rId24" xr:uid="{D327F964-4247-480C-ABF2-CE1C58A5C248}"/>
+    <hyperlink ref="E17" r:id="rId25" xr:uid="{899ABF8F-A4FE-4A5E-81D4-FDAA431DAB0E}"/>
+    <hyperlink ref="E22" r:id="rId26" xr:uid="{DE2CBB3E-53B4-4A72-B17A-95F8DC50A680}"/>
+    <hyperlink ref="E25" r:id="rId27" xr:uid="{5873F399-7F29-4029-A2AF-C59477D7EEFA}"/>
+    <hyperlink ref="E26" r:id="rId28" xr:uid="{9CE1A66B-C3BE-475F-9AAC-35D820A2B426}"/>
+    <hyperlink ref="E27" r:id="rId29" xr:uid="{5442A54E-DEC1-418C-88C0-D3881C3E7DF7}"/>
+    <hyperlink ref="E23" r:id="rId30" xr:uid="{03797E5A-D7A7-48A4-A1B4-62A5C7C463AF}"/>
+    <hyperlink ref="E24" r:id="rId31" xr:uid="{0492AAD8-A54A-4838-943A-8F8C8C981536}"/>
+    <hyperlink ref="E29" r:id="rId32" xr:uid="{D163DA80-AE56-4D17-80D1-BCE62B9B0E77}"/>
+    <hyperlink ref="E35" r:id="rId33" xr:uid="{7EB46669-C518-425D-8A3E-395F05BE96F4}"/>
+    <hyperlink ref="E55" r:id="rId34" xr:uid="{E604A0FD-1B8B-4069-A5D9-749A14F9519E}"/>
+    <hyperlink ref="E56" r:id="rId35" xr:uid="{6D72DCB3-71D9-4096-B636-A24037DEC0A0}"/>
+    <hyperlink ref="E57" r:id="rId36" xr:uid="{F48B074D-BE93-4758-BDD0-50BF937B211E}"/>
+    <hyperlink ref="E8" r:id="rId37" xr:uid="{7F8992C5-905E-4B72-82BE-676D324D1D17}"/>
+    <hyperlink ref="E77" r:id="rId38" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{C875791B-2744-4F5C-9948-8B038AB7B795}"/>
     <hyperlink ref="E29:E42" r:id="rId39" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{CE0B26B0-E940-4BD5-8F74-8D28A4F3B13A}"/>
-    <hyperlink ref="E35" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
-    <hyperlink ref="E53" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
-    <hyperlink ref="E13" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
+    <hyperlink ref="E36" r:id="rId40" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5152B189-9CFA-4B7A-842F-93D4B5F53177}"/>
+    <hyperlink ref="E54" r:id="rId41" display="https://www.coursera.org/verify/LSGX9WZD2829" xr:uid="{5C171493-E45D-436D-968B-6A7D6CED71CA}"/>
+    <hyperlink ref="E14" r:id="rId42" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{CC465E8A-1F75-432D-9DC6-368FD314B682}"/>
     <hyperlink ref="E9:E10" r:id="rId43" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{C55AB7BE-0BE1-4CE1-8CFE-C0E7B2B0BA28}"/>
     <hyperlink ref="E12:E15" r:id="rId44" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{549C4CBA-43AF-4870-BE36-8D1CBC3CFD71}"/>
-    <hyperlink ref="E29" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
-    <hyperlink ref="E61" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
-    <hyperlink ref="E6" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
-    <hyperlink ref="E5" r:id="rId48" display="https://www.hackerrank.com/certificates/eafe133d26dc" xr:uid="{3748E750-A80A-4402-BC5F-803B16F27441}"/>
-    <hyperlink ref="E2" r:id="rId49" xr:uid="{59D89928-3553-4495-8CD7-92EBC3B422E3}"/>
+    <hyperlink ref="E30" r:id="rId45" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{53B8A539-1C54-4D29-828E-465373C8A2C4}"/>
+    <hyperlink ref="E62" r:id="rId46" display="https://www.udemy.com/certificate/UC-cba24dc1-e21d-4c7c-b5b3-1cd55995d707/" xr:uid="{6D2FD0D9-7715-4D27-986B-9CBDCC24BC65}"/>
+    <hyperlink ref="E7" r:id="rId47" xr:uid="{699CE3D0-7418-4EFB-9798-81677CCAC0DE}"/>
+    <hyperlink ref="E6" r:id="rId48" display="https://www.hackerrank.com/certificates/eafe133d26dc" xr:uid="{3748E750-A80A-4402-BC5F-803B16F27441}"/>
+    <hyperlink ref="E3" r:id="rId49" xr:uid="{59D89928-3553-4495-8CD7-92EBC3B422E3}"/>
+    <hyperlink ref="E2" r:id="rId50" xr:uid="{90A10946-4B5C-4200-83CE-B2047CBD914F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3618,27 +3649,27 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>224</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="G1" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="E1" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -3647,73 +3678,73 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="28">
+      <c r="C2" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2" s="27">
         <v>44470</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>230</v>
+      <c r="G2" s="27" t="s">
+        <v>233</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" s="27">
+        <v>44378</v>
+      </c>
+      <c r="G3" s="27">
+        <v>44469</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="F3" s="28">
-        <v>44378</v>
-      </c>
-      <c r="G3" s="28">
-        <v>44469</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>231</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>234</v>
+        <v>238</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>237</v>
       </c>
       <c r="F4" s="20">
         <v>44263</v>
@@ -3722,54 +3753,54 @@
         <v>44377</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" s="34" customFormat="1" ht="75">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:9" s="33" customFormat="1" ht="75">
+      <c r="A5" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>237</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>239</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="E5" s="31" t="s">
+      <c r="F5" s="31">
+        <v>44137</v>
+      </c>
+      <c r="G5" s="31">
+        <v>44200</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="F5" s="32">
-        <v>44137</v>
-      </c>
-      <c r="G5" s="32">
-        <v>44200</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>240</v>
+      <c r="I5" s="32" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>234</v>
+        <v>245</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>237</v>
       </c>
       <c r="F6" s="20">
         <v>44136</v>
@@ -3778,27 +3809,27 @@
         <v>44166</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>234</v>
+      <c r="C7" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>237</v>
       </c>
       <c r="F7" s="20">
         <v>44105</v>
@@ -3807,27 +3838,27 @@
         <v>44136</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>234</v>
+        <v>253</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>237</v>
       </c>
       <c r="F8" s="20">
         <v>43432</v>
@@ -3836,10 +3867,10 @@
         <v>43442</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3906,7 +3937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718451B2-E12D-4ABD-B26C-5975AED3964E}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3915,16 +3946,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>253</v>
+      <c r="A1" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B2" s="7">
         <v>0.9</v>
@@ -3932,7 +3963,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B3" s="7">
         <v>0.8</v>
@@ -3940,7 +3971,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B4" s="7">
         <v>0.8</v>
@@ -3948,7 +3979,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B5" s="7">
         <v>0.8</v>
@@ -3956,7 +3987,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B6" s="7">
         <v>0.8</v>
@@ -3964,7 +3995,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B7" s="7">
         <v>0.8</v>
@@ -3972,7 +4003,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B8" s="7">
         <v>0.8</v>
@@ -3980,7 +4011,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B9" s="7">
         <v>0.7</v>
@@ -3988,7 +4019,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B10" s="7">
         <v>0.7</v>
@@ -3996,7 +4027,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B11" s="7">
         <v>0.7</v>
@@ -4004,7 +4035,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B12" s="7">
         <v>0.7</v>
@@ -4012,7 +4043,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B13" s="7">
         <v>0.6</v>
@@ -4020,7 +4051,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B14" s="7">
         <v>0.6</v>
@@ -4028,7 +4059,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B15" s="7">
         <v>0.6</v>
@@ -4036,7 +4067,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B16" s="7">
         <v>0.6</v>
@@ -4044,7 +4075,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B17" s="7">
         <v>0.6</v>
@@ -4052,7 +4083,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B18" s="7">
         <v>0.6</v>
@@ -4060,7 +4091,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B19" s="7">
         <v>0.6</v>
@@ -4068,7 +4099,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B20" s="7">
         <v>0.5</v>
@@ -4076,7 +4107,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B21" s="7">
         <v>0.5</v>
@@ -4084,7 +4115,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B22" s="7">
         <v>0.5</v>
@@ -4117,199 +4148,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>274</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>275</v>
+      <c r="B1" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -4333,18 +4364,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4565,11 +4596,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F92213D-1611-4A06-8F7F-2A2F3FD54BB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5E4A532-34F4-4909-9773-2D1B4D74CA0C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>